<commit_message>
Solve Exercise 1: Statistics & Simple Regression
</commit_message>
<xml_diff>
--- a/labs/lab7/Lab7_regression_with_excel.xlsx
+++ b/labs/lab7/Lab7_regression_with_excel.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18625"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elias\Dropbox\PSE 2017\PSE and DS 2017\Lab13_regression with excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kasloujr\Desktop\PSEs-and-Data-Science\labs\lab7\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20000" windowHeight="8880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19995" windowHeight="8880"/>
   </bookViews>
   <sheets>
     <sheet name="Simple Regression" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="994" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1024" uniqueCount="104">
   <si>
     <t>PRICE</t>
   </si>
@@ -254,12 +254,96 @@
   <si>
     <t>poor</t>
   </si>
+  <si>
+    <t>SUMMARY OUTPUT</t>
+  </si>
+  <si>
+    <t>Regression Statistics</t>
+  </si>
+  <si>
+    <t>Multiple R</t>
+  </si>
+  <si>
+    <t>R Square</t>
+  </si>
+  <si>
+    <t>Adjusted R Square</t>
+  </si>
+  <si>
+    <t>Standard Error</t>
+  </si>
+  <si>
+    <t>Observations</t>
+  </si>
+  <si>
+    <t>ANOVA</t>
+  </si>
+  <si>
+    <t>Regression</t>
+  </si>
+  <si>
+    <t>Residual</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Intercept</t>
+  </si>
+  <si>
+    <t>df</t>
+  </si>
+  <si>
+    <t>SS</t>
+  </si>
+  <si>
+    <t>MS</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>Significance F</t>
+  </si>
+  <si>
+    <t>Coefficients</t>
+  </si>
+  <si>
+    <t>t Stat</t>
+  </si>
+  <si>
+    <t>P-value</t>
+  </si>
+  <si>
+    <t>Lower 95%</t>
+  </si>
+  <si>
+    <t>Upper 95%</t>
+  </si>
+  <si>
+    <t>Lower 95,0%</t>
+  </si>
+  <si>
+    <t>Upper 95,0%</t>
+  </si>
+  <si>
+    <t>RESIDUAL OUTPUT</t>
+  </si>
+  <si>
+    <t>Observation</t>
+  </si>
+  <si>
+    <t>Predicted PRICE</t>
+  </si>
+  <si>
+    <t>Residuals</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -309,6 +393,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -318,7 +408,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -335,11 +425,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -355,6 +465,14 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -384,7 +502,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{482DAA88-AD68-43DC-9D99-80A1919E2F1B}">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -404,16 +522,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>352425</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>676274</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>47624</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>266699</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>47624</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -428,8 +546,453 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1571625" y="104775"/>
-          <a:ext cx="6724650" cy="5353050"/>
+          <a:off x="7010399" y="4105274"/>
+          <a:ext cx="6810375" cy="6610350"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="2">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Description: </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>The data are a random sample of records of resales of homes from Feb 15 to Apr 30, 1993 from the files maintained by the Albuquerque Board of Realtors. </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400"/>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1400"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>This type of data is collected by multiple listing agencies in many cities and is used by realtors as an information base. </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400"/>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Number of cases: 106 </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400"/>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Variable Names:</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400"/>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="171450" indent="-171450">
+            <a:buFont typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            <a:buChar char="•"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>PRICE = Selling price ($hundreds)</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400"/>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="171450" indent="-171450">
+            <a:buFont typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            <a:buChar char="•"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>SQFT = Square feet of living space</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400"/>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="171450" indent="-171450">
+            <a:buFont typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            <a:buChar char="•"/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" indent="0">
+            <a:buFont typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            <a:buNone/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>a) What linear relationship (model) do you see between the variables? </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Are there any problems with this model? </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>What can you do? Hint: Run a regression of Price on Sqft!</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400"/>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>b) Write the regression equation. What is this equation? How else could you obtain it?</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400"/>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>c) Interpret the intercept and slope coefficient. Do they make sense?</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400"/>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>d) What hypotheses would you set up to test the significance of the slope coefficient at 5% significance level. </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Use both p-value method and Critical value method to conclude.</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400"/>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>e) Predict the price of a house of 2000 SQFT</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400"/>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>f) Interpret the Multiple R of this regression. What other Excel formula/tool can give the same number?</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400"/>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>g) Interpret the coefficient of determinantion.</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400"/>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>114</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="TextBox 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7305675" y="16430625"/>
+          <a:ext cx="6810375" cy="6543675"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3466,23 +4029,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -3518,23 +4064,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -3710,435 +4239,1178 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M107"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N130"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1171875" defaultRowHeight="15.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="3" width="9.1171875" style="1"/>
-    <col min="4" max="4" width="18.41015625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="12.87890625" style="1" customWidth="1"/>
+    <col min="1" max="3" width="9.140625" style="1"/>
+    <col min="4" max="4" width="18.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" style="1" customWidth="1"/>
     <col min="6" max="6" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5859375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="12.41015625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.5859375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.1171875" style="1"/>
+    <col min="7" max="7" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5703125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:14">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="F1" t="s">
+        <v>76</v>
+      </c>
+      <c r="G1"/>
+      <c r="H1"/>
+      <c r="I1"/>
+      <c r="J1"/>
+      <c r="K1"/>
+      <c r="L1"/>
+      <c r="M1"/>
+      <c r="N1"/>
+    </row>
+    <row r="2" spans="1:14" ht="16.5" thickBot="1">
       <c r="A2" s="1">
         <v>2050</v>
       </c>
       <c r="B2" s="1">
         <v>2650</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
+      <c r="F2"/>
+      <c r="G2"/>
+      <c r="H2"/>
+      <c r="I2"/>
+      <c r="J2"/>
+      <c r="K2"/>
+      <c r="L2"/>
+      <c r="M2"/>
+      <c r="N2"/>
+    </row>
+    <row r="3" spans="1:14">
       <c r="A3" s="1">
         <v>2080</v>
       </c>
       <c r="B3" s="1">
         <v>2600</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
+      <c r="F3" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="G3" s="16"/>
+      <c r="H3"/>
+      <c r="I3"/>
+      <c r="J3"/>
+      <c r="K3"/>
+      <c r="L3"/>
+      <c r="M3"/>
+      <c r="N3"/>
+    </row>
+    <row r="4" spans="1:14">
       <c r="A4" s="1">
         <v>2150</v>
       </c>
       <c r="B4" s="1">
         <v>2664</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
+      <c r="F4" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="G4" s="13">
+        <v>0.84116902412069405</v>
+      </c>
+      <c r="H4"/>
+      <c r="I4"/>
+      <c r="J4"/>
+      <c r="K4"/>
+      <c r="L4"/>
+      <c r="M4"/>
+      <c r="N4"/>
+    </row>
+    <row r="5" spans="1:14">
       <c r="A5" s="1">
         <v>2150</v>
       </c>
       <c r="B5" s="1">
         <v>2921</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
+      <c r="F5" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="G5" s="13">
+        <v>0.70756532714016074</v>
+      </c>
+      <c r="H5"/>
+      <c r="I5"/>
+      <c r="J5"/>
+      <c r="K5"/>
+      <c r="L5"/>
+      <c r="M5"/>
+      <c r="N5"/>
+    </row>
+    <row r="6" spans="1:14">
       <c r="A6" s="1">
         <v>1999</v>
       </c>
       <c r="B6" s="1">
         <v>2580</v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
+      <c r="F6" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="G6" s="13">
+        <v>0.70475345528573918</v>
+      </c>
+      <c r="H6"/>
+      <c r="I6"/>
+      <c r="J6"/>
+      <c r="K6"/>
+      <c r="L6"/>
+      <c r="M6"/>
+      <c r="N6"/>
+    </row>
+    <row r="7" spans="1:14">
       <c r="A7" s="1">
         <v>1900</v>
       </c>
       <c r="B7" s="1">
         <v>2580</v>
       </c>
-    </row>
-    <row r="8" spans="1:2">
+      <c r="F7" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="G7" s="13">
+        <v>208.10139841877344</v>
+      </c>
+      <c r="H7"/>
+      <c r="I7"/>
+      <c r="J7"/>
+      <c r="K7"/>
+      <c r="L7"/>
+      <c r="M7"/>
+      <c r="N7"/>
+    </row>
+    <row r="8" spans="1:14" ht="16.5" thickBot="1">
       <c r="A8" s="1">
         <v>1800</v>
       </c>
       <c r="B8" s="1">
         <v>2774</v>
       </c>
-    </row>
-    <row r="9" spans="1:2">
+      <c r="F8" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="G8" s="14">
+        <v>106</v>
+      </c>
+      <c r="H8"/>
+      <c r="I8"/>
+      <c r="J8"/>
+      <c r="K8"/>
+      <c r="L8"/>
+      <c r="M8"/>
+      <c r="N8"/>
+    </row>
+    <row r="9" spans="1:14">
       <c r="A9" s="1">
         <v>1560</v>
       </c>
       <c r="B9" s="1">
         <v>1920</v>
       </c>
-    </row>
-    <row r="10" spans="1:2">
+      <c r="F9"/>
+      <c r="G9"/>
+      <c r="H9"/>
+      <c r="I9"/>
+      <c r="J9"/>
+      <c r="K9"/>
+      <c r="L9"/>
+      <c r="M9"/>
+      <c r="N9"/>
+    </row>
+    <row r="10" spans="1:14" ht="16.5" thickBot="1">
       <c r="A10" s="1">
         <v>1449</v>
       </c>
       <c r="B10" s="1">
         <v>1710</v>
       </c>
-    </row>
-    <row r="11" spans="1:2">
+      <c r="F10" t="s">
+        <v>83</v>
+      </c>
+      <c r="G10"/>
+      <c r="H10"/>
+      <c r="I10"/>
+      <c r="J10"/>
+      <c r="K10"/>
+      <c r="L10"/>
+      <c r="M10"/>
+      <c r="N10"/>
+    </row>
+    <row r="11" spans="1:14">
       <c r="A11" s="1">
         <v>1375</v>
       </c>
       <c r="B11" s="1">
         <v>1837</v>
       </c>
-    </row>
-    <row r="12" spans="1:2">
+      <c r="F11" s="15"/>
+      <c r="G11" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="H11" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="I11" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="J11" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="K11" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="L11"/>
+      <c r="M11"/>
+      <c r="N11"/>
+    </row>
+    <row r="12" spans="1:14">
       <c r="A12" s="1">
         <v>1270</v>
       </c>
       <c r="B12" s="1">
         <v>1880</v>
       </c>
-    </row>
-    <row r="13" spans="1:2">
+      <c r="F12" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="G12" s="13">
+        <v>1</v>
+      </c>
+      <c r="H12" s="13">
+        <v>10897352.906878177</v>
+      </c>
+      <c r="I12" s="13">
+        <v>10897352.906878177</v>
+      </c>
+      <c r="J12" s="13">
+        <v>251.6349833039329</v>
+      </c>
+      <c r="K12" s="13">
+        <v>1.5824121461550127E-29</v>
+      </c>
+      <c r="L12"/>
+      <c r="M12"/>
+      <c r="N12"/>
+    </row>
+    <row r="13" spans="1:14">
       <c r="A13" s="1">
         <v>1250</v>
       </c>
       <c r="B13" s="1">
         <v>2150</v>
       </c>
-    </row>
-    <row r="14" spans="1:2">
+      <c r="F13" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="G13" s="13">
+        <v>104</v>
+      </c>
+      <c r="H13" s="13">
+        <v>4503843.9704803051</v>
+      </c>
+      <c r="I13" s="13">
+        <v>43306.192023849086</v>
+      </c>
+      <c r="J13" s="13"/>
+      <c r="K13" s="13"/>
+      <c r="L13"/>
+      <c r="M13"/>
+      <c r="N13"/>
+    </row>
+    <row r="14" spans="1:14" ht="16.5" thickBot="1">
       <c r="A14" s="1">
         <v>1235</v>
       </c>
       <c r="B14" s="1">
         <v>1894</v>
       </c>
-    </row>
-    <row r="15" spans="1:2">
+      <c r="F14" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="G14" s="14">
+        <v>105</v>
+      </c>
+      <c r="H14" s="14">
+        <v>15401196.877358481</v>
+      </c>
+      <c r="I14" s="14"/>
+      <c r="J14" s="14"/>
+      <c r="K14" s="14"/>
+      <c r="L14"/>
+      <c r="M14"/>
+      <c r="N14"/>
+    </row>
+    <row r="15" spans="1:14" ht="16.5" thickBot="1">
       <c r="A15" s="1">
         <v>1170</v>
       </c>
       <c r="B15" s="1">
         <v>1928</v>
       </c>
-    </row>
-    <row r="16" spans="1:2">
+      <c r="F15"/>
+      <c r="G15"/>
+      <c r="H15"/>
+      <c r="I15"/>
+      <c r="J15"/>
+      <c r="K15"/>
+      <c r="L15"/>
+      <c r="M15"/>
+      <c r="N15"/>
+    </row>
+    <row r="16" spans="1:14">
       <c r="A16" s="1">
         <v>1180</v>
       </c>
       <c r="B16" s="1">
         <v>1830</v>
       </c>
-    </row>
-    <row r="17" spans="1:2">
+      <c r="F16" s="15"/>
+      <c r="G16" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="H16" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="I16" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="J16" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="K16" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="L16" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="M16" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="N16" s="15" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14">
       <c r="A17" s="1">
         <v>1155</v>
       </c>
       <c r="B17" s="1">
         <v>1767</v>
       </c>
-    </row>
-    <row r="18" spans="1:2">
+      <c r="F17" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="G17" s="13">
+        <v>64.956113386531797</v>
+      </c>
+      <c r="H17" s="13">
+        <v>66.675450074977547</v>
+      </c>
+      <c r="I17" s="13">
+        <v>0.97421334709383545</v>
+      </c>
+      <c r="J17" s="13">
+        <v>0.33221115787672917</v>
+      </c>
+      <c r="K17" s="13">
+        <v>-67.263806207341048</v>
+      </c>
+      <c r="L17" s="13">
+        <v>197.17603298040464</v>
+      </c>
+      <c r="M17" s="13">
+        <v>-67.263806207341048</v>
+      </c>
+      <c r="N17" s="13">
+        <v>197.17603298040464</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" ht="16.5" thickBot="1">
       <c r="A18" s="1">
         <v>1110</v>
       </c>
       <c r="B18" s="1">
         <v>1630</v>
       </c>
-    </row>
-    <row r="19" spans="1:2">
+      <c r="F18" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="G18" s="14">
+        <v>0.60635341113087982</v>
+      </c>
+      <c r="H18" s="14">
+        <v>3.8224368211031305E-2</v>
+      </c>
+      <c r="I18" s="14">
+        <v>15.863006754834737</v>
+      </c>
+      <c r="J18" s="14">
+        <v>1.5824121461551253E-29</v>
+      </c>
+      <c r="K18" s="14">
+        <v>0.53055305454227297</v>
+      </c>
+      <c r="L18" s="14">
+        <v>0.68215376771948666</v>
+      </c>
+      <c r="M18" s="14">
+        <v>0.53055305454227297</v>
+      </c>
+      <c r="N18" s="14">
+        <v>0.68215376771948666</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14">
       <c r="A19" s="1">
         <v>1139</v>
       </c>
       <c r="B19" s="1">
         <v>1680</v>
       </c>
-    </row>
-    <row r="20" spans="1:2">
+      <c r="F19"/>
+      <c r="G19"/>
+      <c r="H19"/>
+      <c r="I19"/>
+      <c r="J19"/>
+      <c r="K19"/>
+      <c r="L19"/>
+      <c r="M19"/>
+      <c r="N19"/>
+    </row>
+    <row r="20" spans="1:14">
       <c r="A20" s="1">
         <v>995</v>
       </c>
       <c r="B20" s="1">
         <v>1725</v>
       </c>
-    </row>
-    <row r="21" spans="1:2">
+      <c r="F20"/>
+      <c r="G20"/>
+      <c r="H20"/>
+      <c r="I20"/>
+      <c r="J20"/>
+      <c r="K20"/>
+      <c r="L20"/>
+      <c r="M20"/>
+      <c r="N20"/>
+    </row>
+    <row r="21" spans="1:14">
       <c r="A21" s="1">
         <v>995</v>
       </c>
       <c r="B21" s="1">
         <v>1500</v>
       </c>
-    </row>
-    <row r="22" spans="1:2">
+      <c r="F21"/>
+      <c r="G21"/>
+      <c r="H21"/>
+      <c r="I21"/>
+      <c r="J21"/>
+      <c r="K21"/>
+      <c r="L21"/>
+      <c r="M21"/>
+      <c r="N21"/>
+    </row>
+    <row r="22" spans="1:14">
       <c r="A22" s="1">
         <v>975</v>
       </c>
       <c r="B22" s="1">
         <v>1430</v>
       </c>
-    </row>
-    <row r="23" spans="1:2">
+      <c r="F22" t="s">
+        <v>100</v>
+      </c>
+      <c r="G22"/>
+      <c r="H22"/>
+      <c r="I22"/>
+      <c r="J22"/>
+      <c r="K22"/>
+      <c r="L22"/>
+      <c r="M22"/>
+      <c r="N22"/>
+    </row>
+    <row r="23" spans="1:14" ht="16.5" thickBot="1">
       <c r="A23" s="1">
         <v>975</v>
       </c>
       <c r="B23" s="1">
         <v>1360</v>
       </c>
-    </row>
-    <row r="24" spans="1:2">
+      <c r="F23"/>
+      <c r="G23"/>
+      <c r="H23"/>
+      <c r="I23"/>
+      <c r="J23"/>
+      <c r="K23"/>
+      <c r="L23"/>
+      <c r="M23"/>
+      <c r="N23"/>
+    </row>
+    <row r="24" spans="1:14">
       <c r="A24" s="1">
         <v>900</v>
       </c>
       <c r="B24" s="1">
         <v>1400</v>
       </c>
-    </row>
-    <row r="25" spans="1:2">
+      <c r="F24" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="G24" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="H24" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="I24"/>
+      <c r="J24"/>
+      <c r="K24"/>
+      <c r="L24"/>
+      <c r="M24"/>
+      <c r="N24"/>
+    </row>
+    <row r="25" spans="1:14">
       <c r="A25" s="1">
         <v>960</v>
       </c>
       <c r="B25" s="1">
         <v>1573</v>
       </c>
-    </row>
-    <row r="26" spans="1:2">
+      <c r="F25" s="13">
+        <v>1</v>
+      </c>
+      <c r="G25" s="13">
+        <v>1671.7926528833634</v>
+      </c>
+      <c r="H25" s="13">
+        <v>378.20734711663658</v>
+      </c>
+      <c r="I25"/>
+      <c r="J25"/>
+      <c r="K25"/>
+      <c r="L25"/>
+      <c r="M25"/>
+      <c r="N25"/>
+    </row>
+    <row r="26" spans="1:14">
       <c r="A26" s="1">
         <v>860</v>
       </c>
       <c r="B26" s="1">
         <v>1385</v>
       </c>
-    </row>
-    <row r="27" spans="1:2">
+      <c r="F26" s="13">
+        <v>2</v>
+      </c>
+      <c r="G26" s="13">
+        <v>1641.4749823268194</v>
+      </c>
+      <c r="H26" s="13">
+        <v>438.52501767318063</v>
+      </c>
+      <c r="I26"/>
+      <c r="J26"/>
+      <c r="K26"/>
+      <c r="L26"/>
+      <c r="M26"/>
+      <c r="N26"/>
+    </row>
+    <row r="27" spans="1:14">
       <c r="A27" s="1">
         <v>1695</v>
       </c>
       <c r="B27" s="1">
         <v>2931</v>
       </c>
-    </row>
-    <row r="28" spans="1:2">
+      <c r="F27" s="13">
+        <v>3</v>
+      </c>
+      <c r="G27" s="13">
+        <v>1680.2816006391956</v>
+      </c>
+      <c r="H27" s="13">
+        <v>469.71839936080437</v>
+      </c>
+      <c r="I27"/>
+      <c r="J27"/>
+      <c r="K27"/>
+      <c r="L27"/>
+      <c r="M27"/>
+      <c r="N27"/>
+    </row>
+    <row r="28" spans="1:14">
       <c r="A28" s="1">
         <v>1300</v>
       </c>
       <c r="B28" s="1">
         <v>2000</v>
       </c>
-    </row>
-    <row r="29" spans="1:2">
+      <c r="F28" s="13">
+        <v>4</v>
+      </c>
+      <c r="G28" s="13">
+        <v>1836.1144272998317</v>
+      </c>
+      <c r="H28" s="13">
+        <v>313.88557270016827</v>
+      </c>
+      <c r="I28"/>
+      <c r="J28"/>
+      <c r="K28"/>
+      <c r="L28"/>
+      <c r="M28"/>
+      <c r="N28"/>
+    </row>
+    <row r="29" spans="1:14">
       <c r="A29" s="1">
         <v>1020</v>
       </c>
       <c r="B29" s="1">
         <v>1478</v>
       </c>
-    </row>
-    <row r="30" spans="1:2">
+      <c r="F29" s="13">
+        <v>5</v>
+      </c>
+      <c r="G29" s="13">
+        <v>1629.3479141042017</v>
+      </c>
+      <c r="H29" s="13">
+        <v>369.65208589579834</v>
+      </c>
+      <c r="I29"/>
+      <c r="J29"/>
+      <c r="K29"/>
+      <c r="L29"/>
+      <c r="M29"/>
+      <c r="N29"/>
+    </row>
+    <row r="30" spans="1:14">
       <c r="A30" s="1">
         <v>1020</v>
       </c>
       <c r="B30" s="1">
         <v>1713</v>
       </c>
-    </row>
-    <row r="31" spans="1:2">
+      <c r="F30" s="13">
+        <v>6</v>
+      </c>
+      <c r="G30" s="13">
+        <v>1629.3479141042017</v>
+      </c>
+      <c r="H30" s="13">
+        <v>270.65208589579834</v>
+      </c>
+      <c r="I30"/>
+      <c r="J30"/>
+      <c r="K30"/>
+      <c r="L30"/>
+      <c r="M30"/>
+      <c r="N30"/>
+    </row>
+    <row r="31" spans="1:14">
       <c r="A31" s="1">
         <v>922</v>
       </c>
       <c r="B31" s="1">
         <v>1326</v>
       </c>
-    </row>
-    <row r="32" spans="1:2">
+      <c r="F31" s="13">
+        <v>7</v>
+      </c>
+      <c r="G31" s="13">
+        <v>1746.9804758635923</v>
+      </c>
+      <c r="H31" s="13">
+        <v>53.019524136407654</v>
+      </c>
+      <c r="I31"/>
+      <c r="J31"/>
+      <c r="K31"/>
+      <c r="L31"/>
+      <c r="M31"/>
+      <c r="N31"/>
+    </row>
+    <row r="32" spans="1:14">
       <c r="A32" s="1">
         <v>925</v>
       </c>
       <c r="B32" s="1">
         <v>1050</v>
       </c>
-    </row>
-    <row r="33" spans="1:2">
+      <c r="F32" s="13">
+        <v>8</v>
+      </c>
+      <c r="G32" s="13">
+        <v>1229.1546627578211</v>
+      </c>
+      <c r="H32" s="13">
+        <v>330.84533724217886</v>
+      </c>
+      <c r="I32"/>
+      <c r="J32"/>
+      <c r="K32"/>
+      <c r="L32"/>
+      <c r="M32"/>
+      <c r="N32"/>
+    </row>
+    <row r="33" spans="1:14">
       <c r="A33" s="1">
         <v>899</v>
       </c>
       <c r="B33" s="1">
         <v>1464</v>
       </c>
-    </row>
-    <row r="34" spans="1:2">
+      <c r="F33" s="13">
+        <v>9</v>
+      </c>
+      <c r="G33" s="13">
+        <v>1101.8204464203363</v>
+      </c>
+      <c r="H33" s="13">
+        <v>347.17955357966366</v>
+      </c>
+      <c r="I33"/>
+      <c r="J33"/>
+      <c r="K33"/>
+      <c r="L33"/>
+      <c r="M33"/>
+      <c r="N33"/>
+    </row>
+    <row r="34" spans="1:14">
       <c r="A34" s="1">
         <v>850</v>
       </c>
       <c r="B34" s="1">
         <v>1190</v>
       </c>
-    </row>
-    <row r="35" spans="1:2">
+      <c r="F34" s="13">
+        <v>10</v>
+      </c>
+      <c r="G34" s="13">
+        <v>1178.827329633958</v>
+      </c>
+      <c r="H34" s="13">
+        <v>196.17267036604198</v>
+      </c>
+      <c r="I34"/>
+      <c r="J34"/>
+      <c r="K34"/>
+      <c r="L34"/>
+      <c r="M34"/>
+      <c r="N34"/>
+    </row>
+    <row r="35" spans="1:14">
       <c r="A35" s="1">
         <v>890</v>
       </c>
       <c r="B35" s="1">
         <v>1746</v>
       </c>
-    </row>
-    <row r="36" spans="1:2">
+      <c r="F35" s="13">
+        <v>11</v>
+      </c>
+      <c r="G35" s="13">
+        <v>1204.900526312586</v>
+      </c>
+      <c r="H35" s="13">
+        <v>65.099473687414047</v>
+      </c>
+      <c r="I35"/>
+      <c r="J35"/>
+      <c r="K35"/>
+      <c r="L35"/>
+      <c r="M35"/>
+      <c r="N35"/>
+    </row>
+    <row r="36" spans="1:14">
       <c r="A36" s="1">
         <v>870</v>
       </c>
       <c r="B36" s="1">
         <v>1280</v>
       </c>
-    </row>
-    <row r="37" spans="1:2">
+      <c r="F36" s="13">
+        <v>12</v>
+      </c>
+      <c r="G36" s="13">
+        <v>1368.6159473179234</v>
+      </c>
+      <c r="H36" s="13">
+        <v>-118.61594731792343</v>
+      </c>
+      <c r="I36"/>
+      <c r="J36"/>
+      <c r="K36"/>
+      <c r="L36"/>
+      <c r="M36"/>
+      <c r="N36"/>
+    </row>
+    <row r="37" spans="1:14">
       <c r="A37" s="1">
         <v>700</v>
       </c>
       <c r="B37" s="1">
         <v>1215</v>
       </c>
-    </row>
-    <row r="38" spans="1:2">
+      <c r="F37" s="13">
+        <v>13</v>
+      </c>
+      <c r="G37" s="13">
+        <v>1213.3894740684182</v>
+      </c>
+      <c r="H37" s="13">
+        <v>21.610525931581833</v>
+      </c>
+      <c r="I37"/>
+      <c r="J37"/>
+      <c r="K37"/>
+      <c r="L37"/>
+      <c r="M37"/>
+      <c r="N37"/>
+    </row>
+    <row r="38" spans="1:14">
       <c r="A38" s="1">
         <v>720</v>
       </c>
       <c r="B38" s="1">
         <v>1121</v>
       </c>
-    </row>
-    <row r="39" spans="1:2">
+      <c r="F38" s="13">
+        <v>14</v>
+      </c>
+      <c r="G38" s="13">
+        <v>1234.0054900468681</v>
+      </c>
+      <c r="H38" s="13">
+        <v>-64.00549004686809</v>
+      </c>
+      <c r="I38"/>
+      <c r="J38"/>
+      <c r="K38"/>
+      <c r="L38"/>
+      <c r="M38"/>
+      <c r="N38"/>
+    </row>
+    <row r="39" spans="1:14">
       <c r="A39" s="1">
         <v>749</v>
       </c>
       <c r="B39" s="1">
         <v>1733</v>
       </c>
-    </row>
-    <row r="40" spans="1:2">
+      <c r="F39" s="13">
+        <v>15</v>
+      </c>
+      <c r="G39" s="13">
+        <v>1174.5828557560419</v>
+      </c>
+      <c r="H39" s="13">
+        <v>5.4171442439580915</v>
+      </c>
+      <c r="I39"/>
+      <c r="J39"/>
+      <c r="K39"/>
+      <c r="L39"/>
+      <c r="M39"/>
+      <c r="N39"/>
+    </row>
+    <row r="40" spans="1:14">
       <c r="A40" s="1">
         <v>731</v>
       </c>
       <c r="B40" s="1">
         <v>1299</v>
       </c>
-    </row>
-    <row r="41" spans="1:2">
+      <c r="F40" s="13">
+        <v>16</v>
+      </c>
+      <c r="G40" s="13">
+        <v>1136.3825908547965</v>
+      </c>
+      <c r="H40" s="13">
+        <v>18.61740914520351</v>
+      </c>
+      <c r="I40"/>
+      <c r="J40"/>
+      <c r="K40"/>
+      <c r="L40"/>
+      <c r="M40"/>
+      <c r="N40"/>
+    </row>
+    <row r="41" spans="1:14">
       <c r="A41" s="1">
         <v>725</v>
       </c>
       <c r="B41" s="1">
         <v>1140</v>
       </c>
-    </row>
-    <row r="42" spans="1:2">
+      <c r="F41" s="13">
+        <v>17</v>
+      </c>
+      <c r="G41" s="13">
+        <v>1053.312173529866</v>
+      </c>
+      <c r="H41" s="13">
+        <v>56.687826470134041</v>
+      </c>
+      <c r="I41"/>
+      <c r="J41"/>
+      <c r="K41"/>
+      <c r="L41"/>
+      <c r="M41"/>
+      <c r="N41"/>
+    </row>
+    <row r="42" spans="1:14">
       <c r="A42" s="1">
         <v>670</v>
       </c>
       <c r="B42" s="1">
         <v>1181</v>
       </c>
-    </row>
-    <row r="43" spans="1:2">
+      <c r="F42" s="13">
+        <v>18</v>
+      </c>
+      <c r="G42" s="13">
+        <v>1083.6298440864098</v>
+      </c>
+      <c r="H42" s="13">
+        <v>55.370155913590224</v>
+      </c>
+      <c r="I42"/>
+      <c r="J42"/>
+      <c r="K42"/>
+      <c r="L42"/>
+      <c r="M42"/>
+      <c r="N42"/>
+    </row>
+    <row r="43" spans="1:14">
       <c r="A43" s="1">
         <v>2150</v>
       </c>
       <c r="B43" s="1">
         <v>2848</v>
       </c>
-    </row>
-    <row r="44" spans="1:2">
+      <c r="F43" s="13">
+        <v>19</v>
+      </c>
+      <c r="G43" s="13">
+        <v>1110.9157475872994</v>
+      </c>
+      <c r="H43" s="13">
+        <v>-115.91574758729939</v>
+      </c>
+      <c r="I43"/>
+      <c r="J43"/>
+      <c r="K43"/>
+      <c r="L43"/>
+      <c r="M43"/>
+      <c r="N43"/>
+    </row>
+    <row r="44" spans="1:14">
       <c r="A44" s="1">
         <v>1599</v>
       </c>
       <c r="B44" s="1">
         <v>2440</v>
       </c>
-    </row>
-    <row r="45" spans="1:2">
+      <c r="F44" s="13">
+        <v>20</v>
+      </c>
+      <c r="G44" s="13">
+        <v>974.48623008285153</v>
+      </c>
+      <c r="H44" s="13">
+        <v>20.513769917148466</v>
+      </c>
+      <c r="I44"/>
+      <c r="J44"/>
+      <c r="K44"/>
+      <c r="L44"/>
+      <c r="M44"/>
+      <c r="N44"/>
+    </row>
+    <row r="45" spans="1:14">
       <c r="A45" s="1">
         <v>1350</v>
       </c>
       <c r="B45" s="1">
         <v>2253</v>
       </c>
-    </row>
-    <row r="46" spans="1:2">
+      <c r="F45" s="13">
+        <v>21</v>
+      </c>
+      <c r="G45" s="13">
+        <v>932.0414913036899</v>
+      </c>
+      <c r="H45" s="13">
+        <v>42.958508696310105</v>
+      </c>
+      <c r="I45"/>
+      <c r="J45"/>
+      <c r="K45"/>
+      <c r="L45"/>
+      <c r="M45"/>
+      <c r="N45"/>
+    </row>
+    <row r="46" spans="1:14">
       <c r="A46" s="1">
         <v>1299</v>
       </c>
       <c r="B46" s="1">
         <v>2743</v>
       </c>
-    </row>
-    <row r="47" spans="1:2">
+      <c r="F46" s="13">
+        <v>22</v>
+      </c>
+      <c r="G46" s="13">
+        <v>889.59675252452837</v>
+      </c>
+      <c r="H46" s="13">
+        <v>85.40324747547163</v>
+      </c>
+      <c r="I46"/>
+      <c r="J46"/>
+      <c r="K46"/>
+      <c r="L46"/>
+      <c r="M46"/>
+      <c r="N46"/>
+    </row>
+    <row r="47" spans="1:14">
       <c r="A47" s="1">
         <v>1250</v>
       </c>
       <c r="B47" s="1">
         <v>2180</v>
       </c>
-    </row>
-    <row r="48" spans="1:2">
+      <c r="F47" s="13">
+        <v>23</v>
+      </c>
+      <c r="G47" s="13">
+        <v>913.85088896976356</v>
+      </c>
+      <c r="H47" s="13">
+        <v>-13.85088896976356</v>
+      </c>
+      <c r="I47"/>
+      <c r="J47"/>
+      <c r="K47"/>
+      <c r="L47"/>
+      <c r="M47"/>
+      <c r="N47"/>
+    </row>
+    <row r="48" spans="1:14">
       <c r="A48" s="1">
         <v>1239</v>
       </c>
       <c r="B48" s="1">
         <v>1706</v>
       </c>
-    </row>
-    <row r="49" spans="1:13">
+      <c r="F48" s="13">
+        <v>24</v>
+      </c>
+      <c r="G48" s="13">
+        <v>1018.7500290954057</v>
+      </c>
+      <c r="H48" s="13">
+        <v>-58.750029095405694</v>
+      </c>
+      <c r="I48"/>
+      <c r="J48"/>
+      <c r="K48"/>
+      <c r="L48"/>
+      <c r="M48"/>
+      <c r="N48"/>
+    </row>
+    <row r="49" spans="1:14">
       <c r="A49" s="1">
         <v>1200</v>
       </c>
       <c r="B49" s="1">
         <v>1948</v>
       </c>
-    </row>
-    <row r="50" spans="1:13">
+      <c r="F49" s="13">
+        <v>25</v>
+      </c>
+      <c r="G49" s="13">
+        <v>904.75558780280039</v>
+      </c>
+      <c r="H49" s="13">
+        <v>-44.755587802800392</v>
+      </c>
+      <c r="I49"/>
+      <c r="J49"/>
+      <c r="K49"/>
+      <c r="L49"/>
+      <c r="M49"/>
+      <c r="N49"/>
+    </row>
+    <row r="50" spans="1:14">
       <c r="A50" s="1">
         <v>1125</v>
       </c>
       <c r="B50" s="1">
         <v>1710</v>
       </c>
-    </row>
-    <row r="51" spans="1:13">
+      <c r="F50" s="13">
+        <v>26</v>
+      </c>
+      <c r="G50" s="13">
+        <v>1842.1779614111406</v>
+      </c>
+      <c r="H50" s="13">
+        <v>-147.17796141114059</v>
+      </c>
+      <c r="I50"/>
+      <c r="J50"/>
+      <c r="K50"/>
+      <c r="L50"/>
+      <c r="M50"/>
+      <c r="N50"/>
+    </row>
+    <row r="51" spans="1:14">
       <c r="A51" s="1">
         <v>1100</v>
       </c>
       <c r="B51" s="1">
         <v>1657</v>
       </c>
-    </row>
-    <row r="52" spans="1:13">
+      <c r="F51" s="13">
+        <v>27</v>
+      </c>
+      <c r="G51" s="13">
+        <v>1277.6629356482915</v>
+      </c>
+      <c r="H51" s="13">
+        <v>22.337064351708477</v>
+      </c>
+      <c r="I51"/>
+      <c r="J51"/>
+      <c r="K51"/>
+      <c r="L51"/>
+      <c r="M51"/>
+      <c r="N51"/>
+    </row>
+    <row r="52" spans="1:14">
       <c r="A52" s="1">
         <v>1080</v>
       </c>
@@ -4146,16 +5418,23 @@
         <v>2200</v>
       </c>
       <c r="E52" s="2"/>
-      <c r="F52" s="2"/>
-      <c r="G52" s="2"/>
-      <c r="H52" s="2"/>
-      <c r="I52" s="2"/>
-      <c r="J52" s="2"/>
-      <c r="K52" s="2"/>
-      <c r="L52" s="2"/>
-      <c r="M52" s="2"/>
-    </row>
-    <row r="53" spans="1:13">
+      <c r="F52" s="13">
+        <v>28</v>
+      </c>
+      <c r="G52" s="13">
+        <v>961.14645503797215</v>
+      </c>
+      <c r="H52" s="13">
+        <v>58.853544962027854</v>
+      </c>
+      <c r="I52"/>
+      <c r="J52"/>
+      <c r="K52"/>
+      <c r="L52"/>
+      <c r="M52"/>
+      <c r="N52"/>
+    </row>
+    <row r="53" spans="1:14">
       <c r="A53" s="1">
         <v>1050</v>
       </c>
@@ -4163,16 +5442,23 @@
         <v>1680</v>
       </c>
       <c r="E53" s="3"/>
-      <c r="F53" s="3"/>
-      <c r="G53" s="3"/>
-      <c r="H53" s="3"/>
-      <c r="I53" s="3"/>
-      <c r="J53" s="3"/>
-      <c r="K53" s="3"/>
-      <c r="L53" s="3"/>
-      <c r="M53" s="3"/>
-    </row>
-    <row r="54" spans="1:13">
+      <c r="F53" s="13">
+        <v>29</v>
+      </c>
+      <c r="G53" s="13">
+        <v>1103.6395066537289</v>
+      </c>
+      <c r="H53" s="13">
+        <v>-83.639506653728859</v>
+      </c>
+      <c r="I53"/>
+      <c r="J53"/>
+      <c r="K53"/>
+      <c r="L53"/>
+      <c r="M53"/>
+      <c r="N53"/>
+    </row>
+    <row r="54" spans="1:14">
       <c r="A54" s="1">
         <v>1049</v>
       </c>
@@ -4180,16 +5466,23 @@
         <v>1900</v>
       </c>
       <c r="E54" s="3"/>
-      <c r="F54" s="3"/>
-      <c r="G54" s="3"/>
-      <c r="H54" s="3"/>
-      <c r="I54" s="3"/>
-      <c r="J54" s="3"/>
-      <c r="K54" s="3"/>
-      <c r="L54" s="3"/>
-      <c r="M54" s="3"/>
-    </row>
-    <row r="55" spans="1:13">
+      <c r="F54" s="13">
+        <v>30</v>
+      </c>
+      <c r="G54" s="13">
+        <v>868.98073654607845</v>
+      </c>
+      <c r="H54" s="13">
+        <v>53.019263453921553</v>
+      </c>
+      <c r="I54"/>
+      <c r="J54"/>
+      <c r="K54"/>
+      <c r="L54"/>
+      <c r="M54"/>
+      <c r="N54"/>
+    </row>
+    <row r="55" spans="1:14">
       <c r="A55" s="1">
         <v>955</v>
       </c>
@@ -4197,430 +5490,1608 @@
         <v>1565</v>
       </c>
       <c r="E55" s="3"/>
-      <c r="F55" s="3"/>
-      <c r="G55" s="3"/>
-      <c r="H55" s="3"/>
-      <c r="I55" s="3"/>
-      <c r="J55" s="3"/>
-      <c r="K55" s="3"/>
-      <c r="L55" s="3"/>
-      <c r="M55" s="3"/>
-    </row>
-    <row r="56" spans="1:13">
+      <c r="F55" s="13">
+        <v>31</v>
+      </c>
+      <c r="G55" s="13">
+        <v>701.62719507395559</v>
+      </c>
+      <c r="H55" s="13">
+        <v>223.37280492604441</v>
+      </c>
+      <c r="I55"/>
+      <c r="J55"/>
+      <c r="K55"/>
+      <c r="L55"/>
+      <c r="M55"/>
+      <c r="N55"/>
+    </row>
+    <row r="56" spans="1:14">
       <c r="A56" s="1">
         <v>934</v>
       </c>
       <c r="B56" s="1">
         <v>1543</v>
       </c>
-    </row>
-    <row r="57" spans="1:13">
+      <c r="F56" s="13">
+        <v>32</v>
+      </c>
+      <c r="G56" s="13">
+        <v>952.65750728213982</v>
+      </c>
+      <c r="H56" s="13">
+        <v>-53.657507282139818</v>
+      </c>
+      <c r="I56"/>
+      <c r="J56"/>
+      <c r="K56"/>
+      <c r="L56"/>
+      <c r="M56"/>
+      <c r="N56"/>
+    </row>
+    <row r="57" spans="1:14">
       <c r="A57" s="1">
         <v>875</v>
       </c>
       <c r="B57" s="1">
         <v>1173</v>
       </c>
-    </row>
-    <row r="58" spans="1:13">
+      <c r="F57" s="13">
+        <v>33</v>
+      </c>
+      <c r="G57" s="13">
+        <v>786.51667263227876</v>
+      </c>
+      <c r="H57" s="13">
+        <v>63.483327367721245</v>
+      </c>
+      <c r="I57"/>
+      <c r="J57"/>
+      <c r="K57"/>
+      <c r="L57"/>
+      <c r="M57"/>
+      <c r="N57"/>
+    </row>
+    <row r="58" spans="1:14">
       <c r="A58" s="1">
         <v>889</v>
       </c>
       <c r="B58" s="1">
         <v>1549</v>
       </c>
-    </row>
-    <row r="59" spans="1:13">
+      <c r="F58" s="13">
+        <v>34</v>
+      </c>
+      <c r="G58" s="13">
+        <v>1123.6491692210479</v>
+      </c>
+      <c r="H58" s="13">
+        <v>-233.64916922104794</v>
+      </c>
+      <c r="I58"/>
+      <c r="J58"/>
+      <c r="K58"/>
+      <c r="L58"/>
+      <c r="M58"/>
+      <c r="N58"/>
+    </row>
+    <row r="59" spans="1:14">
       <c r="A59" s="1">
         <v>855</v>
       </c>
       <c r="B59" s="1">
         <v>1900</v>
       </c>
-    </row>
-    <row r="60" spans="1:13">
+      <c r="F59" s="13">
+        <v>35</v>
+      </c>
+      <c r="G59" s="13">
+        <v>841.08847963405799</v>
+      </c>
+      <c r="H59" s="13">
+        <v>28.91152036594201</v>
+      </c>
+      <c r="I59"/>
+      <c r="J59"/>
+      <c r="K59"/>
+      <c r="L59"/>
+      <c r="M59"/>
+      <c r="N59"/>
+    </row>
+    <row r="60" spans="1:14">
       <c r="A60" s="1">
         <v>835</v>
       </c>
       <c r="B60" s="1">
         <v>1560</v>
       </c>
-    </row>
-    <row r="61" spans="1:13">
+      <c r="F60" s="13">
+        <v>36</v>
+      </c>
+      <c r="G60" s="13">
+        <v>801.67550791055078</v>
+      </c>
+      <c r="H60" s="13">
+        <v>-101.67550791055078</v>
+      </c>
+      <c r="I60"/>
+      <c r="J60"/>
+      <c r="K60"/>
+      <c r="L60"/>
+      <c r="M60"/>
+      <c r="N60"/>
+    </row>
+    <row r="61" spans="1:14">
       <c r="A61" s="1">
         <v>810</v>
       </c>
       <c r="B61" s="1">
         <v>1365</v>
       </c>
-    </row>
-    <row r="62" spans="1:13">
+      <c r="F61" s="13">
+        <v>37</v>
+      </c>
+      <c r="G61" s="13">
+        <v>744.67828726424807</v>
+      </c>
+      <c r="H61" s="13">
+        <v>-24.67828726424807</v>
+      </c>
+      <c r="I61"/>
+      <c r="J61"/>
+      <c r="K61"/>
+      <c r="L61"/>
+      <c r="M61"/>
+      <c r="N61"/>
+    </row>
+    <row r="62" spans="1:14">
       <c r="A62" s="1">
         <v>805</v>
       </c>
       <c r="B62" s="1">
         <v>1258</v>
       </c>
-    </row>
-    <row r="63" spans="1:13">
+      <c r="F62" s="13">
+        <v>38</v>
+      </c>
+      <c r="G62" s="13">
+        <v>1115.7665748763466</v>
+      </c>
+      <c r="H62" s="13">
+        <v>-366.76657487634657</v>
+      </c>
+      <c r="I62"/>
+      <c r="J62"/>
+      <c r="K62"/>
+      <c r="L62"/>
+      <c r="M62"/>
+      <c r="N62"/>
+    </row>
+    <row r="63" spans="1:14">
       <c r="A63" s="1">
         <v>799</v>
       </c>
       <c r="B63" s="1">
         <v>1314</v>
       </c>
-    </row>
-    <row r="64" spans="1:13">
+      <c r="F63" s="13">
+        <v>39</v>
+      </c>
+      <c r="G63" s="13">
+        <v>852.60919444554463</v>
+      </c>
+      <c r="H63" s="13">
+        <v>-121.60919444554463</v>
+      </c>
+      <c r="I63"/>
+      <c r="J63"/>
+      <c r="K63"/>
+      <c r="L63"/>
+      <c r="M63"/>
+      <c r="N63"/>
+    </row>
+    <row r="64" spans="1:14">
       <c r="A64" s="1">
         <v>750</v>
       </c>
       <c r="B64" s="1">
         <v>1338</v>
       </c>
-    </row>
-    <row r="65" spans="1:2">
+      <c r="F64" s="13">
+        <v>40</v>
+      </c>
+      <c r="G64" s="13">
+        <v>756.19900207573482</v>
+      </c>
+      <c r="H64" s="13">
+        <v>-31.199002075734825</v>
+      </c>
+      <c r="I64"/>
+      <c r="J64"/>
+      <c r="K64"/>
+      <c r="L64"/>
+      <c r="M64"/>
+      <c r="N64"/>
+    </row>
+    <row r="65" spans="1:14">
       <c r="A65" s="1">
         <v>759</v>
       </c>
       <c r="B65" s="1">
         <v>997</v>
       </c>
-    </row>
-    <row r="66" spans="1:2">
+      <c r="F65" s="13">
+        <v>41</v>
+      </c>
+      <c r="G65" s="13">
+        <v>781.05949193210085</v>
+      </c>
+      <c r="H65" s="13">
+        <v>-111.05949193210085</v>
+      </c>
+      <c r="I65"/>
+      <c r="J65"/>
+      <c r="K65"/>
+      <c r="L65"/>
+      <c r="M65"/>
+      <c r="N65"/>
+    </row>
+    <row r="66" spans="1:14">
       <c r="A66" s="1">
         <v>750</v>
       </c>
       <c r="B66" s="1">
         <v>1030</v>
       </c>
-    </row>
-    <row r="67" spans="1:2">
+      <c r="F66" s="13">
+        <v>42</v>
+      </c>
+      <c r="G66" s="13">
+        <v>1791.8506282872775</v>
+      </c>
+      <c r="H66" s="13">
+        <v>358.14937171272254</v>
+      </c>
+      <c r="I66"/>
+      <c r="J66"/>
+      <c r="K66"/>
+      <c r="L66"/>
+      <c r="M66"/>
+      <c r="N66"/>
+    </row>
+    <row r="67" spans="1:14">
       <c r="A67" s="1">
         <v>730</v>
       </c>
       <c r="B67" s="1">
         <v>1027</v>
       </c>
-    </row>
-    <row r="68" spans="1:2">
+      <c r="F67" s="13">
+        <v>43</v>
+      </c>
+      <c r="G67" s="13">
+        <v>1544.4584365458786</v>
+      </c>
+      <c r="H67" s="13">
+        <v>54.541563454121388</v>
+      </c>
+      <c r="I67"/>
+      <c r="J67"/>
+      <c r="K67"/>
+      <c r="L67"/>
+      <c r="M67"/>
+      <c r="N67"/>
+    </row>
+    <row r="68" spans="1:14">
       <c r="A68" s="1">
         <v>729</v>
       </c>
       <c r="B68" s="1">
         <v>1007</v>
       </c>
-    </row>
-    <row r="69" spans="1:2">
+      <c r="F68" s="13">
+        <v>44</v>
+      </c>
+      <c r="G68" s="13">
+        <v>1431.070348664404</v>
+      </c>
+      <c r="H68" s="13">
+        <v>-81.070348664404037</v>
+      </c>
+      <c r="I68"/>
+      <c r="J68"/>
+      <c r="K68"/>
+      <c r="L68"/>
+      <c r="M68"/>
+      <c r="N68"/>
+    </row>
+    <row r="69" spans="1:14">
       <c r="A69" s="1">
         <v>710</v>
       </c>
       <c r="B69" s="1">
         <v>1083</v>
       </c>
-    </row>
-    <row r="70" spans="1:2">
+      <c r="F69" s="13">
+        <v>45</v>
+      </c>
+      <c r="G69" s="13">
+        <v>1728.1835201185352</v>
+      </c>
+      <c r="H69" s="13">
+        <v>-429.18352011853517</v>
+      </c>
+      <c r="I69"/>
+      <c r="J69"/>
+      <c r="K69"/>
+      <c r="L69"/>
+      <c r="M69"/>
+      <c r="N69"/>
+    </row>
+    <row r="70" spans="1:14">
       <c r="A70" s="1">
         <v>670</v>
       </c>
       <c r="B70" s="1">
         <v>1350</v>
       </c>
-    </row>
-    <row r="71" spans="1:2">
+      <c r="F70" s="13">
+        <v>46</v>
+      </c>
+      <c r="G70" s="13">
+        <v>1386.8065496518498</v>
+      </c>
+      <c r="H70" s="13">
+        <v>-136.80654965184976</v>
+      </c>
+      <c r="I70"/>
+      <c r="J70"/>
+      <c r="K70"/>
+      <c r="L70"/>
+      <c r="M70"/>
+      <c r="N70"/>
+    </row>
+    <row r="71" spans="1:14">
       <c r="A71" s="1">
         <v>619</v>
       </c>
       <c r="B71" s="1">
         <v>837</v>
       </c>
-    </row>
-    <row r="72" spans="1:2">
+      <c r="F71" s="13">
+        <v>47</v>
+      </c>
+      <c r="G71" s="13">
+        <v>1099.3950327758128</v>
+      </c>
+      <c r="H71" s="13">
+        <v>139.60496722418725</v>
+      </c>
+      <c r="I71"/>
+      <c r="J71"/>
+      <c r="K71"/>
+      <c r="L71"/>
+      <c r="M71"/>
+      <c r="N71"/>
+    </row>
+    <row r="72" spans="1:14">
       <c r="A72" s="1">
         <v>1295</v>
       </c>
       <c r="B72" s="1">
         <v>3750</v>
       </c>
-    </row>
-    <row r="73" spans="1:2">
+      <c r="F72" s="13">
+        <v>48</v>
+      </c>
+      <c r="G72" s="13">
+        <v>1246.1325582694856</v>
+      </c>
+      <c r="H72" s="13">
+        <v>-46.132558269485571</v>
+      </c>
+      <c r="I72"/>
+      <c r="J72"/>
+      <c r="K72"/>
+      <c r="L72"/>
+      <c r="M72"/>
+      <c r="N72"/>
+    </row>
+    <row r="73" spans="1:14">
       <c r="A73" s="1">
         <v>975</v>
       </c>
       <c r="B73" s="1">
         <v>1500</v>
       </c>
-    </row>
-    <row r="74" spans="1:2">
+      <c r="F73" s="13">
+        <v>49</v>
+      </c>
+      <c r="G73" s="13">
+        <v>1101.8204464203363</v>
+      </c>
+      <c r="H73" s="13">
+        <v>23.179553579663661</v>
+      </c>
+      <c r="I73"/>
+      <c r="J73"/>
+      <c r="K73"/>
+      <c r="L73"/>
+      <c r="M73"/>
+      <c r="N73"/>
+    </row>
+    <row r="74" spans="1:14">
       <c r="A74" s="1">
         <v>939</v>
       </c>
       <c r="B74" s="1">
         <v>1428</v>
       </c>
-    </row>
-    <row r="75" spans="1:2">
+      <c r="F74" s="13">
+        <v>50</v>
+      </c>
+      <c r="G74" s="13">
+        <v>1069.6837156303995</v>
+      </c>
+      <c r="H74" s="13">
+        <v>30.316284369600453</v>
+      </c>
+      <c r="I74"/>
+      <c r="J74"/>
+      <c r="K74"/>
+      <c r="L74"/>
+      <c r="M74"/>
+      <c r="N74"/>
+    </row>
+    <row r="75" spans="1:14">
       <c r="A75" s="1">
         <v>820</v>
       </c>
       <c r="B75" s="1">
         <v>1375</v>
       </c>
-    </row>
-    <row r="76" spans="1:2">
+      <c r="F75" s="13">
+        <v>51</v>
+      </c>
+      <c r="G75" s="13">
+        <v>1398.9336178744675</v>
+      </c>
+      <c r="H75" s="13">
+        <v>-318.93361787446747</v>
+      </c>
+      <c r="I75"/>
+      <c r="J75"/>
+      <c r="K75"/>
+      <c r="L75"/>
+      <c r="M75"/>
+      <c r="N75"/>
+    </row>
+    <row r="76" spans="1:14">
       <c r="A76" s="1">
         <v>780</v>
       </c>
       <c r="B76" s="1">
         <v>1080</v>
       </c>
-    </row>
-    <row r="77" spans="1:2">
+      <c r="F76" s="13">
+        <v>52</v>
+      </c>
+      <c r="G76" s="13">
+        <v>1083.6298440864098</v>
+      </c>
+      <c r="H76" s="13">
+        <v>-33.629844086409776</v>
+      </c>
+      <c r="I76"/>
+      <c r="J76"/>
+      <c r="K76"/>
+      <c r="L76"/>
+      <c r="M76"/>
+      <c r="N76"/>
+    </row>
+    <row r="77" spans="1:14">
       <c r="A77" s="1">
         <v>770</v>
       </c>
       <c r="B77" s="1">
         <v>900</v>
       </c>
-    </row>
-    <row r="78" spans="1:2">
+      <c r="F77" s="13">
+        <v>53</v>
+      </c>
+      <c r="G77" s="13">
+        <v>1217.0275945352034</v>
+      </c>
+      <c r="H77" s="13">
+        <v>-168.02759453520343</v>
+      </c>
+      <c r="I77"/>
+      <c r="J77"/>
+      <c r="K77"/>
+      <c r="L77"/>
+      <c r="M77"/>
+      <c r="N77"/>
+    </row>
+    <row r="78" spans="1:14">
       <c r="A78" s="1">
         <v>700</v>
       </c>
       <c r="B78" s="1">
         <v>1505</v>
       </c>
-    </row>
-    <row r="79" spans="1:2">
+      <c r="F78" s="13">
+        <v>54</v>
+      </c>
+      <c r="G78" s="13">
+        <v>1013.8992018063587</v>
+      </c>
+      <c r="H78" s="13">
+        <v>-58.899201806358747</v>
+      </c>
+      <c r="I78"/>
+      <c r="J78"/>
+      <c r="K78"/>
+      <c r="L78"/>
+      <c r="M78"/>
+      <c r="N78"/>
+    </row>
+    <row r="79" spans="1:14">
       <c r="A79" s="1">
         <v>540</v>
       </c>
       <c r="B79" s="1">
         <v>1142</v>
       </c>
-    </row>
-    <row r="80" spans="1:2">
+      <c r="F79" s="13">
+        <v>55</v>
+      </c>
+      <c r="G79" s="13">
+        <v>1000.5594267614794</v>
+      </c>
+      <c r="H79" s="13">
+        <v>-66.559426761479358</v>
+      </c>
+      <c r="I79"/>
+      <c r="J79"/>
+      <c r="K79"/>
+      <c r="L79"/>
+      <c r="M79"/>
+      <c r="N79"/>
+    </row>
+    <row r="80" spans="1:14">
       <c r="A80" s="1">
         <v>1070</v>
       </c>
       <c r="B80" s="1">
         <v>1464</v>
       </c>
-    </row>
-    <row r="81" spans="1:2">
+      <c r="F80" s="13">
+        <v>56</v>
+      </c>
+      <c r="G80" s="13">
+        <v>776.20866464305379</v>
+      </c>
+      <c r="H80" s="13">
+        <v>98.791335356946206</v>
+      </c>
+      <c r="I80"/>
+      <c r="J80"/>
+      <c r="K80"/>
+      <c r="L80"/>
+      <c r="M80"/>
+      <c r="N80"/>
+    </row>
+    <row r="81" spans="1:14">
       <c r="A81" s="1">
         <v>2100</v>
       </c>
       <c r="B81" s="1">
         <v>2116</v>
       </c>
-    </row>
-    <row r="82" spans="1:2">
+      <c r="F81" s="13">
+        <v>57</v>
+      </c>
+      <c r="G81" s="13">
+        <v>1004.1975472282646</v>
+      </c>
+      <c r="H81" s="13">
+        <v>-115.19754722826463</v>
+      </c>
+      <c r="I81"/>
+      <c r="J81"/>
+      <c r="K81"/>
+      <c r="L81"/>
+      <c r="M81"/>
+      <c r="N81"/>
+    </row>
+    <row r="82" spans="1:14">
       <c r="A82" s="1">
         <v>725</v>
       </c>
       <c r="B82" s="1">
         <v>1280</v>
       </c>
-    </row>
-    <row r="83" spans="1:2">
+      <c r="F82" s="13">
+        <v>58</v>
+      </c>
+      <c r="G82" s="13">
+        <v>1217.0275945352034</v>
+      </c>
+      <c r="H82" s="13">
+        <v>-362.02759453520343</v>
+      </c>
+      <c r="I82"/>
+      <c r="J82"/>
+      <c r="K82"/>
+      <c r="L82"/>
+      <c r="M82"/>
+      <c r="N82"/>
+    </row>
+    <row r="83" spans="1:14">
       <c r="A83" s="1">
         <v>660</v>
       </c>
       <c r="B83" s="1">
         <v>1159</v>
       </c>
-    </row>
-    <row r="84" spans="1:2">
+      <c r="F83" s="13">
+        <v>59</v>
+      </c>
+      <c r="G83" s="13">
+        <v>1010.8674347507043</v>
+      </c>
+      <c r="H83" s="13">
+        <v>-175.86743475070432</v>
+      </c>
+      <c r="I83"/>
+      <c r="J83"/>
+      <c r="K83"/>
+      <c r="L83"/>
+      <c r="M83"/>
+      <c r="N83"/>
+    </row>
+    <row r="84" spans="1:14">
       <c r="A84" s="1">
         <v>580</v>
       </c>
       <c r="B84" s="1">
         <v>1051</v>
       </c>
-    </row>
-    <row r="85" spans="1:2">
+      <c r="F84" s="13">
+        <v>60</v>
+      </c>
+      <c r="G84" s="13">
+        <v>892.6285195801828</v>
+      </c>
+      <c r="H84" s="13">
+        <v>-82.628519580182797</v>
+      </c>
+      <c r="I84"/>
+      <c r="J84"/>
+      <c r="K84"/>
+      <c r="L84"/>
+      <c r="M84"/>
+      <c r="N84"/>
+    </row>
+    <row r="85" spans="1:14">
       <c r="A85" s="1">
         <v>1844</v>
       </c>
       <c r="B85" s="1">
         <v>2250</v>
       </c>
-    </row>
-    <row r="86" spans="1:2">
+      <c r="F85" s="13">
+        <v>61</v>
+      </c>
+      <c r="G85" s="13">
+        <v>827.7487045891786</v>
+      </c>
+      <c r="H85" s="13">
+        <v>-22.748704589178601</v>
+      </c>
+      <c r="I85"/>
+      <c r="J85"/>
+      <c r="K85"/>
+      <c r="L85"/>
+      <c r="M85"/>
+      <c r="N85"/>
+    </row>
+    <row r="86" spans="1:14">
       <c r="A86" s="1">
         <v>1580</v>
       </c>
       <c r="B86" s="1">
         <v>2563</v>
       </c>
-    </row>
-    <row r="87" spans="1:2">
+      <c r="F86" s="13">
+        <v>62</v>
+      </c>
+      <c r="G86" s="13">
+        <v>861.70449561250791</v>
+      </c>
+      <c r="H86" s="13">
+        <v>-62.704495612507912</v>
+      </c>
+      <c r="I86"/>
+      <c r="J86"/>
+      <c r="K86"/>
+      <c r="L86"/>
+      <c r="M86"/>
+      <c r="N86"/>
+    </row>
+    <row r="87" spans="1:14">
       <c r="A87" s="1">
         <v>699</v>
       </c>
       <c r="B87" s="1">
         <v>1400</v>
       </c>
-    </row>
-    <row r="88" spans="1:2">
+      <c r="F87" s="13">
+        <v>63</v>
+      </c>
+      <c r="G87" s="13">
+        <v>876.25697747964898</v>
+      </c>
+      <c r="H87" s="13">
+        <v>-126.25697747964898</v>
+      </c>
+      <c r="I87"/>
+      <c r="J87"/>
+      <c r="K87"/>
+      <c r="L87"/>
+      <c r="M87"/>
+      <c r="N87"/>
+    </row>
+    <row r="88" spans="1:14">
       <c r="A88" s="1">
         <v>1160</v>
       </c>
       <c r="B88" s="1">
         <v>1720</v>
       </c>
-    </row>
-    <row r="89" spans="1:2">
+      <c r="F88" s="13">
+        <v>64</v>
+      </c>
+      <c r="G88" s="13">
+        <v>669.49046428401903</v>
+      </c>
+      <c r="H88" s="13">
+        <v>89.509535715980974</v>
+      </c>
+      <c r="I88"/>
+      <c r="J88"/>
+      <c r="K88"/>
+      <c r="L88"/>
+      <c r="M88"/>
+      <c r="N88"/>
+    </row>
+    <row r="89" spans="1:14">
       <c r="A89" s="1">
         <v>1109</v>
       </c>
       <c r="B89" s="1">
         <v>1740</v>
       </c>
-    </row>
-    <row r="90" spans="1:2">
+      <c r="F89" s="13">
+        <v>65</v>
+      </c>
+      <c r="G89" s="13">
+        <v>689.500126851338</v>
+      </c>
+      <c r="H89" s="13">
+        <v>60.499873148662004</v>
+      </c>
+      <c r="I89"/>
+      <c r="J89"/>
+      <c r="K89"/>
+      <c r="L89"/>
+      <c r="M89"/>
+      <c r="N89"/>
+    </row>
+    <row r="90" spans="1:14">
       <c r="A90" s="1">
         <v>1129</v>
       </c>
       <c r="B90" s="1">
         <v>1700</v>
       </c>
-    </row>
-    <row r="91" spans="1:2">
+      <c r="F90" s="13">
+        <v>66</v>
+      </c>
+      <c r="G90" s="13">
+        <v>687.68106661794536</v>
+      </c>
+      <c r="H90" s="13">
+        <v>42.318933382054638</v>
+      </c>
+      <c r="I90"/>
+      <c r="J90"/>
+      <c r="K90"/>
+      <c r="L90"/>
+      <c r="M90"/>
+      <c r="N90"/>
+    </row>
+    <row r="91" spans="1:14">
       <c r="A91" s="1">
         <v>1050</v>
       </c>
       <c r="B91" s="1">
         <v>1620</v>
       </c>
-    </row>
-    <row r="92" spans="1:2">
+      <c r="F91" s="13">
+        <v>67</v>
+      </c>
+      <c r="G91" s="13">
+        <v>675.55399839532777</v>
+      </c>
+      <c r="H91" s="13">
+        <v>53.446001604672233</v>
+      </c>
+      <c r="I91"/>
+      <c r="J91"/>
+      <c r="K91"/>
+      <c r="L91"/>
+      <c r="M91"/>
+      <c r="N91"/>
+    </row>
+    <row r="92" spans="1:14">
       <c r="A92" s="1">
         <v>1045</v>
       </c>
       <c r="B92" s="1">
         <v>1630</v>
       </c>
-    </row>
-    <row r="93" spans="1:2">
+      <c r="F92" s="13">
+        <v>68</v>
+      </c>
+      <c r="G92" s="13">
+        <v>721.63685764127467</v>
+      </c>
+      <c r="H92" s="13">
+        <v>-11.636857641274673</v>
+      </c>
+      <c r="I92"/>
+      <c r="J92"/>
+      <c r="K92"/>
+      <c r="L92"/>
+      <c r="M92"/>
+      <c r="N92"/>
+    </row>
+    <row r="93" spans="1:14">
       <c r="A93" s="1">
         <v>1050</v>
       </c>
       <c r="B93" s="1">
         <v>1920</v>
       </c>
-    </row>
-    <row r="94" spans="1:2">
+      <c r="F93" s="13">
+        <v>69</v>
+      </c>
+      <c r="G93" s="13">
+        <v>883.53321841321952</v>
+      </c>
+      <c r="H93" s="13">
+        <v>-213.53321841321952</v>
+      </c>
+      <c r="I93"/>
+      <c r="J93"/>
+      <c r="K93"/>
+      <c r="L93"/>
+      <c r="M93"/>
+      <c r="N93"/>
+    </row>
+    <row r="94" spans="1:14">
       <c r="A94" s="1">
         <v>1020</v>
       </c>
       <c r="B94" s="1">
         <v>1606</v>
       </c>
-    </row>
-    <row r="95" spans="1:2">
+      <c r="F94" s="13">
+        <v>70</v>
+      </c>
+      <c r="G94" s="13">
+        <v>572.47391850307827</v>
+      </c>
+      <c r="H94" s="13">
+        <v>46.526081496921734</v>
+      </c>
+      <c r="I94"/>
+      <c r="J94"/>
+      <c r="K94"/>
+      <c r="L94"/>
+      <c r="M94"/>
+      <c r="N94"/>
+    </row>
+    <row r="95" spans="1:14">
       <c r="A95" s="1">
         <v>1000</v>
       </c>
       <c r="B95" s="1">
         <v>1535</v>
       </c>
-    </row>
-    <row r="96" spans="1:2">
+      <c r="F95" s="13">
+        <v>71</v>
+      </c>
+      <c r="G95" s="13">
+        <v>2338.7814051273313</v>
+      </c>
+      <c r="H95" s="13">
+        <v>-1043.7814051273313</v>
+      </c>
+      <c r="I95"/>
+      <c r="J95"/>
+      <c r="K95"/>
+      <c r="L95"/>
+      <c r="M95"/>
+      <c r="N95"/>
+    </row>
+    <row r="96" spans="1:14">
       <c r="A96" s="1">
         <v>1030</v>
       </c>
       <c r="B96" s="1">
         <v>1540</v>
       </c>
-    </row>
-    <row r="97" spans="1:2">
+      <c r="F96" s="13">
+        <v>72</v>
+      </c>
+      <c r="G96" s="13">
+        <v>974.48623008285153</v>
+      </c>
+      <c r="H96" s="13">
+        <v>0.51376991714846554</v>
+      </c>
+      <c r="I96"/>
+      <c r="J96"/>
+      <c r="K96"/>
+      <c r="L96"/>
+      <c r="M96"/>
+      <c r="N96"/>
+    </row>
+    <row r="97" spans="1:14">
       <c r="A97" s="1">
         <v>975</v>
       </c>
       <c r="B97" s="1">
         <v>1739</v>
       </c>
-    </row>
-    <row r="98" spans="1:2">
+      <c r="F97" s="13">
+        <v>73</v>
+      </c>
+      <c r="G97" s="13">
+        <v>930.82878448142822</v>
+      </c>
+      <c r="H97" s="13">
+        <v>8.1712155185717847</v>
+      </c>
+      <c r="I97"/>
+      <c r="J97"/>
+      <c r="K97"/>
+      <c r="L97"/>
+      <c r="M97"/>
+      <c r="N97"/>
+    </row>
+    <row r="98" spans="1:14">
       <c r="A98" s="1">
         <v>950</v>
       </c>
       <c r="B98" s="1">
         <v>1715</v>
       </c>
-    </row>
-    <row r="99" spans="1:2">
+      <c r="F98" s="13">
+        <v>74</v>
+      </c>
+      <c r="G98" s="13">
+        <v>898.69205369149154</v>
+      </c>
+      <c r="H98" s="13">
+        <v>-78.692053691491537</v>
+      </c>
+      <c r="I98"/>
+      <c r="J98"/>
+      <c r="K98"/>
+      <c r="L98"/>
+      <c r="M98"/>
+      <c r="N98"/>
+    </row>
+    <row r="99" spans="1:14">
       <c r="A99" s="1">
         <v>940</v>
       </c>
       <c r="B99" s="1">
         <v>1305</v>
       </c>
-    </row>
-    <row r="100" spans="1:2">
+      <c r="F99" s="13">
+        <v>75</v>
+      </c>
+      <c r="G99" s="13">
+        <v>719.81779740788204</v>
+      </c>
+      <c r="H99" s="13">
+        <v>60.18220259211796</v>
+      </c>
+      <c r="I99"/>
+      <c r="J99"/>
+      <c r="K99"/>
+      <c r="L99"/>
+      <c r="M99"/>
+      <c r="N99"/>
+    </row>
+    <row r="100" spans="1:14">
       <c r="A100" s="1">
         <v>920</v>
       </c>
       <c r="B100" s="1">
         <v>1415</v>
       </c>
-    </row>
-    <row r="101" spans="1:2">
+      <c r="F100" s="13">
+        <v>76</v>
+      </c>
+      <c r="G100" s="13">
+        <v>610.67418340432368</v>
+      </c>
+      <c r="H100" s="13">
+        <v>159.32581659567632</v>
+      </c>
+      <c r="I100"/>
+      <c r="J100"/>
+      <c r="K100"/>
+      <c r="L100"/>
+      <c r="M100"/>
+      <c r="N100"/>
+    </row>
+    <row r="101" spans="1:14">
       <c r="A101" s="1">
         <v>945</v>
       </c>
       <c r="B101" s="1">
         <v>1580</v>
       </c>
-    </row>
-    <row r="102" spans="1:2">
+      <c r="F101" s="13">
+        <v>77</v>
+      </c>
+      <c r="G101" s="13">
+        <v>977.51799713850596</v>
+      </c>
+      <c r="H101" s="13">
+        <v>-277.51799713850596</v>
+      </c>
+      <c r="I101"/>
+      <c r="J101"/>
+      <c r="K101"/>
+      <c r="L101"/>
+      <c r="M101"/>
+      <c r="N101"/>
+    </row>
+    <row r="102" spans="1:14">
       <c r="A102" s="1">
         <v>874</v>
       </c>
       <c r="B102" s="1">
         <v>1236</v>
       </c>
-    </row>
-    <row r="103" spans="1:2">
+      <c r="F102" s="13">
+        <v>78</v>
+      </c>
+      <c r="G102" s="13">
+        <v>757.4117088979965</v>
+      </c>
+      <c r="H102" s="13">
+        <v>-217.4117088979965</v>
+      </c>
+      <c r="I102"/>
+      <c r="J102"/>
+      <c r="K102"/>
+      <c r="L102"/>
+      <c r="M102"/>
+      <c r="N102"/>
+    </row>
+    <row r="103" spans="1:14">
       <c r="A103" s="1">
         <v>872</v>
       </c>
       <c r="B103" s="1">
         <v>1229</v>
       </c>
-    </row>
-    <row r="104" spans="1:2">
+      <c r="F103" s="13">
+        <v>79</v>
+      </c>
+      <c r="G103" s="13">
+        <v>952.65750728213982</v>
+      </c>
+      <c r="H103" s="13">
+        <v>117.34249271786018</v>
+      </c>
+      <c r="I103"/>
+      <c r="J103"/>
+      <c r="K103"/>
+      <c r="L103"/>
+      <c r="M103"/>
+      <c r="N103"/>
+    </row>
+    <row r="104" spans="1:14">
       <c r="A104" s="1">
         <v>870</v>
       </c>
       <c r="B104" s="1">
         <v>1273</v>
       </c>
-    </row>
-    <row r="105" spans="1:2">
+      <c r="F104" s="13">
+        <v>80</v>
+      </c>
+      <c r="G104" s="13">
+        <v>1347.9999313394735</v>
+      </c>
+      <c r="H104" s="13">
+        <v>752.00006866052649</v>
+      </c>
+      <c r="I104"/>
+      <c r="J104"/>
+      <c r="K104"/>
+      <c r="L104"/>
+      <c r="M104"/>
+      <c r="N104"/>
+    </row>
+    <row r="105" spans="1:14">
       <c r="A105" s="1">
         <v>869</v>
       </c>
       <c r="B105" s="1">
         <v>1165</v>
       </c>
-    </row>
-    <row r="106" spans="1:2">
+      <c r="F105" s="13">
+        <v>81</v>
+      </c>
+      <c r="G105" s="13">
+        <v>841.08847963405799</v>
+      </c>
+      <c r="H105" s="13">
+        <v>-116.08847963405799</v>
+      </c>
+      <c r="I105"/>
+      <c r="J105"/>
+      <c r="K105"/>
+      <c r="L105"/>
+      <c r="M105"/>
+      <c r="N105"/>
+    </row>
+    <row r="106" spans="1:14">
       <c r="A106" s="1">
         <v>766</v>
       </c>
       <c r="B106" s="1">
         <v>1200</v>
       </c>
-    </row>
-    <row r="107" spans="1:2">
+      <c r="F106" s="13">
+        <v>82</v>
+      </c>
+      <c r="G106" s="13">
+        <v>767.71971688722147</v>
+      </c>
+      <c r="H106" s="13">
+        <v>-107.71971688722147</v>
+      </c>
+      <c r="I106"/>
+      <c r="J106"/>
+      <c r="K106"/>
+      <c r="L106"/>
+      <c r="M106"/>
+      <c r="N106"/>
+    </row>
+    <row r="107" spans="1:14">
       <c r="A107" s="1">
         <v>739</v>
       </c>
       <c r="B107" s="1">
         <v>970</v>
       </c>
+      <c r="F107" s="13">
+        <v>83</v>
+      </c>
+      <c r="G107" s="13">
+        <v>702.23354848508643</v>
+      </c>
+      <c r="H107" s="13">
+        <v>-122.23354848508643</v>
+      </c>
+      <c r="I107"/>
+      <c r="J107"/>
+      <c r="K107"/>
+      <c r="L107"/>
+      <c r="M107"/>
+      <c r="N107"/>
+    </row>
+    <row r="108" spans="1:14">
+      <c r="F108" s="13">
+        <v>84</v>
+      </c>
+      <c r="G108" s="13">
+        <v>1429.2512884310113</v>
+      </c>
+      <c r="H108" s="13">
+        <v>414.74871156898871</v>
+      </c>
+      <c r="I108"/>
+      <c r="J108"/>
+      <c r="K108"/>
+      <c r="L108"/>
+      <c r="M108"/>
+      <c r="N108"/>
+    </row>
+    <row r="109" spans="1:14">
+      <c r="F109" s="13">
+        <v>85</v>
+      </c>
+      <c r="G109" s="13">
+        <v>1619.0399061149767</v>
+      </c>
+      <c r="H109" s="13">
+        <v>-39.039906114976702</v>
+      </c>
+      <c r="I109"/>
+      <c r="J109"/>
+      <c r="K109"/>
+      <c r="L109"/>
+      <c r="M109"/>
+      <c r="N109"/>
+    </row>
+    <row r="110" spans="1:14">
+      <c r="F110" s="13">
+        <v>86</v>
+      </c>
+      <c r="G110" s="13">
+        <v>913.85088896976356</v>
+      </c>
+      <c r="H110" s="13">
+        <v>-214.85088896976356</v>
+      </c>
+      <c r="I110"/>
+      <c r="J110"/>
+      <c r="K110"/>
+      <c r="L110"/>
+      <c r="M110"/>
+      <c r="N110"/>
+    </row>
+    <row r="111" spans="1:14">
+      <c r="F111" s="13">
+        <v>87</v>
+      </c>
+      <c r="G111" s="13">
+        <v>1107.8839805316452</v>
+      </c>
+      <c r="H111" s="13">
+        <v>52.116019468354807</v>
+      </c>
+      <c r="I111"/>
+      <c r="J111"/>
+      <c r="K111"/>
+      <c r="L111"/>
+      <c r="M111"/>
+      <c r="N111"/>
+    </row>
+    <row r="112" spans="1:14">
+      <c r="F112" s="13">
+        <v>88</v>
+      </c>
+      <c r="G112" s="13">
+        <v>1120.0110487542627</v>
+      </c>
+      <c r="H112" s="13">
+        <v>-11.011048754262674</v>
+      </c>
+      <c r="I112"/>
+      <c r="J112"/>
+      <c r="K112"/>
+      <c r="L112"/>
+      <c r="M112"/>
+      <c r="N112"/>
+    </row>
+    <row r="113" spans="6:14">
+      <c r="F113" s="13">
+        <v>89</v>
+      </c>
+      <c r="G113" s="13">
+        <v>1095.7569123090275</v>
+      </c>
+      <c r="H113" s="13">
+        <v>33.243087690972516</v>
+      </c>
+      <c r="I113"/>
+      <c r="J113"/>
+      <c r="K113"/>
+      <c r="L113"/>
+      <c r="M113"/>
+      <c r="N113"/>
+    </row>
+    <row r="114" spans="6:14">
+      <c r="F114" s="13">
+        <v>90</v>
+      </c>
+      <c r="G114" s="13">
+        <v>1047.2486394185571</v>
+      </c>
+      <c r="H114" s="13">
+        <v>2.7513605814428956</v>
+      </c>
+      <c r="I114"/>
+      <c r="J114"/>
+      <c r="K114"/>
+      <c r="L114"/>
+      <c r="M114"/>
+      <c r="N114"/>
+    </row>
+    <row r="115" spans="6:14">
+      <c r="F115" s="13">
+        <v>91</v>
+      </c>
+      <c r="G115" s="13">
+        <v>1053.312173529866</v>
+      </c>
+      <c r="H115" s="13">
+        <v>-8.3121735298659587</v>
+      </c>
+      <c r="I115"/>
+      <c r="J115"/>
+      <c r="K115"/>
+      <c r="L115"/>
+      <c r="M115"/>
+      <c r="N115"/>
+    </row>
+    <row r="116" spans="6:14">
+      <c r="F116" s="13">
+        <v>92</v>
+      </c>
+      <c r="G116" s="13">
+        <v>1229.1546627578211</v>
+      </c>
+      <c r="H116" s="13">
+        <v>-179.15466275782114</v>
+      </c>
+      <c r="I116"/>
+      <c r="J116"/>
+      <c r="K116"/>
+      <c r="L116"/>
+      <c r="M116"/>
+      <c r="N116"/>
+    </row>
+    <row r="117" spans="6:14">
+      <c r="F117" s="13">
+        <v>93</v>
+      </c>
+      <c r="G117" s="13">
+        <v>1038.7596916627249</v>
+      </c>
+      <c r="H117" s="13">
+        <v>-18.75969166272489</v>
+      </c>
+      <c r="I117"/>
+      <c r="J117"/>
+      <c r="K117"/>
+      <c r="L117"/>
+      <c r="M117"/>
+      <c r="N117"/>
+    </row>
+    <row r="118" spans="6:14">
+      <c r="F118" s="13">
+        <v>94</v>
+      </c>
+      <c r="G118" s="13">
+        <v>995.7085994724323</v>
+      </c>
+      <c r="H118" s="13">
+        <v>4.2914005275677027</v>
+      </c>
+      <c r="I118"/>
+      <c r="J118"/>
+      <c r="K118"/>
+      <c r="L118"/>
+      <c r="M118"/>
+      <c r="N118"/>
+    </row>
+    <row r="119" spans="6:14">
+      <c r="F119" s="13">
+        <v>95</v>
+      </c>
+      <c r="G119" s="13">
+        <v>998.74036652808672</v>
+      </c>
+      <c r="H119" s="13">
+        <v>31.259633471913276</v>
+      </c>
+      <c r="I119"/>
+      <c r="J119"/>
+      <c r="K119"/>
+      <c r="L119"/>
+      <c r="M119"/>
+      <c r="N119"/>
+    </row>
+    <row r="120" spans="6:14">
+      <c r="F120" s="13">
+        <v>96</v>
+      </c>
+      <c r="G120" s="13">
+        <v>1119.4046953431318</v>
+      </c>
+      <c r="H120" s="13">
+        <v>-144.40469534313183</v>
+      </c>
+      <c r="I120"/>
+      <c r="J120"/>
+      <c r="K120"/>
+      <c r="L120"/>
+      <c r="M120"/>
+      <c r="N120"/>
+    </row>
+    <row r="121" spans="6:14">
+      <c r="F121" s="13">
+        <v>97</v>
+      </c>
+      <c r="G121" s="13">
+        <v>1104.8522134759908</v>
+      </c>
+      <c r="H121" s="13">
+        <v>-154.85221347599077</v>
+      </c>
+      <c r="I121"/>
+      <c r="J121"/>
+      <c r="K121"/>
+      <c r="L121"/>
+      <c r="M121"/>
+      <c r="N121"/>
+    </row>
+    <row r="122" spans="6:14">
+      <c r="F122" s="13">
+        <v>98</v>
+      </c>
+      <c r="G122" s="13">
+        <v>856.24731491233001</v>
+      </c>
+      <c r="H122" s="13">
+        <v>83.752685087669988</v>
+      </c>
+      <c r="I122"/>
+      <c r="J122"/>
+      <c r="K122"/>
+      <c r="L122"/>
+      <c r="M122"/>
+      <c r="N122"/>
+    </row>
+    <row r="123" spans="6:14">
+      <c r="F123" s="13">
+        <v>99</v>
+      </c>
+      <c r="G123" s="13">
+        <v>922.94619013672673</v>
+      </c>
+      <c r="H123" s="13">
+        <v>-2.9461901367267274</v>
+      </c>
+      <c r="I123"/>
+      <c r="J123"/>
+      <c r="K123"/>
+      <c r="L123"/>
+      <c r="M123"/>
+      <c r="N123"/>
+    </row>
+    <row r="124" spans="6:14">
+      <c r="F124" s="13">
+        <v>100</v>
+      </c>
+      <c r="G124" s="13">
+        <v>1022.9945029733219</v>
+      </c>
+      <c r="H124" s="13">
+        <v>-77.994502973321914</v>
+      </c>
+      <c r="I124"/>
+      <c r="J124"/>
+      <c r="K124"/>
+      <c r="L124"/>
+      <c r="M124"/>
+      <c r="N124"/>
+    </row>
+    <row r="125" spans="6:14">
+      <c r="F125" s="13">
+        <v>101</v>
+      </c>
+      <c r="G125" s="13">
+        <v>814.40892954429921</v>
+      </c>
+      <c r="H125" s="13">
+        <v>59.591070455700788</v>
+      </c>
+      <c r="I125"/>
+      <c r="J125"/>
+      <c r="K125"/>
+      <c r="L125"/>
+      <c r="M125"/>
+      <c r="N125"/>
+    </row>
+    <row r="126" spans="6:14">
+      <c r="F126" s="13">
+        <v>102</v>
+      </c>
+      <c r="G126" s="13">
+        <v>810.16445566638311</v>
+      </c>
+      <c r="H126" s="13">
+        <v>61.835544333616895</v>
+      </c>
+      <c r="I126"/>
+      <c r="J126"/>
+      <c r="K126"/>
+      <c r="L126"/>
+      <c r="M126"/>
+      <c r="N126"/>
+    </row>
+    <row r="127" spans="6:14">
+      <c r="F127" s="13">
+        <v>103</v>
+      </c>
+      <c r="G127" s="13">
+        <v>836.84400575614177</v>
+      </c>
+      <c r="H127" s="13">
+        <v>33.155994243858231</v>
+      </c>
+      <c r="I127"/>
+      <c r="J127"/>
+      <c r="K127"/>
+      <c r="L127"/>
+      <c r="M127"/>
+      <c r="N127"/>
+    </row>
+    <row r="128" spans="6:14">
+      <c r="F128" s="13">
+        <v>104</v>
+      </c>
+      <c r="G128" s="13">
+        <v>771.35783735400673</v>
+      </c>
+      <c r="H128" s="13">
+        <v>97.642162645993267</v>
+      </c>
+      <c r="I128"/>
+      <c r="J128"/>
+      <c r="K128"/>
+      <c r="L128"/>
+      <c r="M128"/>
+      <c r="N128"/>
+    </row>
+    <row r="129" spans="6:14">
+      <c r="F129" s="13">
+        <v>105</v>
+      </c>
+      <c r="G129" s="13">
+        <v>792.58020674358761</v>
+      </c>
+      <c r="H129" s="13">
+        <v>-26.58020674358761</v>
+      </c>
+      <c r="I129"/>
+      <c r="J129"/>
+      <c r="K129"/>
+      <c r="L129"/>
+      <c r="M129"/>
+      <c r="N129"/>
+    </row>
+    <row r="130" spans="6:14" ht="16.5" thickBot="1">
+      <c r="F130" s="14">
+        <v>106</v>
+      </c>
+      <c r="G130" s="14">
+        <v>653.11892218348521</v>
+      </c>
+      <c r="H130" s="14">
+        <v>85.881077816514789</v>
+      </c>
+      <c r="I130"/>
+      <c r="J130"/>
+      <c r="K130"/>
+      <c r="L130"/>
+      <c r="M130"/>
+      <c r="N130"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -4632,21 +7103,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="L43" sqref="L43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.7"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="10.29296875" customWidth="1"/>
-    <col min="2" max="2" width="22.87890625" customWidth="1"/>
+    <col min="1" max="1" width="10.28515625" customWidth="1"/>
+    <col min="2" max="2" width="22.85546875" customWidth="1"/>
     <col min="3" max="3" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="13.7">
+    <row r="1" spans="1:5" ht="15">
       <c r="A1" s="9" t="s">
         <v>2</v>
       </c>
@@ -5477,26 +7948,26 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="L37" sqref="L37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1171875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="3.87890625" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.29296875" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5859375" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.29296875" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5859375" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="9.1171875" style="4"/>
-    <col min="9" max="9" width="12.5859375" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.1171875" style="4"/>
+    <col min="1" max="1" width="3.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="9.140625" style="4"/>
+    <col min="9" max="9" width="12.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.35">
+    <row r="1" spans="1:10" ht="15.75">
       <c r="A1" s="10" t="s">
         <v>57</v>
       </c>
@@ -5518,7 +7989,7 @@
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
     </row>
-    <row r="2" spans="1:10" ht="15.35">
+    <row r="2" spans="1:10" ht="15.75">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -5540,7 +8011,7 @@
       <c r="I2" s="5"/>
       <c r="J2" s="5"/>
     </row>
-    <row r="3" spans="1:10" ht="15.35">
+    <row r="3" spans="1:10" ht="15.75">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -5562,7 +8033,7 @@
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
     </row>
-    <row r="4" spans="1:10" ht="15.35">
+    <row r="4" spans="1:10" ht="15.75">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -5584,7 +8055,7 @@
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
     </row>
-    <row r="5" spans="1:10" ht="15.35">
+    <row r="5" spans="1:10" ht="15.75">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -5606,7 +8077,7 @@
       <c r="I5" s="5"/>
       <c r="J5" s="5"/>
     </row>
-    <row r="6" spans="1:10" ht="15.35">
+    <row r="6" spans="1:10" ht="15.75">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -5628,7 +8099,7 @@
       <c r="I6" s="5"/>
       <c r="J6" s="5"/>
     </row>
-    <row r="7" spans="1:10" ht="15.35">
+    <row r="7" spans="1:10" ht="15.75">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -5650,7 +8121,7 @@
       <c r="I7" s="5"/>
       <c r="J7" s="5"/>
     </row>
-    <row r="8" spans="1:10" ht="15.35">
+    <row r="8" spans="1:10" ht="15.75">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -5672,7 +8143,7 @@
       <c r="I8" s="5"/>
       <c r="J8" s="5"/>
     </row>
-    <row r="9" spans="1:10" ht="15.35">
+    <row r="9" spans="1:10" ht="15.75">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -5694,7 +8165,7 @@
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
     </row>
-    <row r="10" spans="1:10" ht="15.35">
+    <row r="10" spans="1:10" ht="15.75">
       <c r="A10" s="5">
         <v>9</v>
       </c>
@@ -5716,7 +8187,7 @@
       <c r="I10" s="5"/>
       <c r="J10" s="5"/>
     </row>
-    <row r="11" spans="1:10" ht="15.35">
+    <row r="11" spans="1:10" ht="15.75">
       <c r="A11" s="5">
         <v>10</v>
       </c>
@@ -5738,7 +8209,7 @@
       <c r="I11" s="5"/>
       <c r="J11" s="5"/>
     </row>
-    <row r="12" spans="1:10" ht="15.35">
+    <row r="12" spans="1:10" ht="15.75">
       <c r="A12" s="5">
         <v>11</v>
       </c>
@@ -5760,7 +8231,7 @@
       <c r="I12" s="5"/>
       <c r="J12" s="5"/>
     </row>
-    <row r="13" spans="1:10" ht="15.35">
+    <row r="13" spans="1:10" ht="15.75">
       <c r="A13" s="5">
         <v>12</v>
       </c>
@@ -5782,7 +8253,7 @@
       <c r="I13" s="5"/>
       <c r="J13" s="5"/>
     </row>
-    <row r="14" spans="1:10" ht="15.35">
+    <row r="14" spans="1:10" ht="15.75">
       <c r="A14" s="5">
         <v>13</v>
       </c>
@@ -5804,7 +8275,7 @@
       <c r="I14" s="5"/>
       <c r="J14" s="5"/>
     </row>
-    <row r="15" spans="1:10" ht="15.35">
+    <row r="15" spans="1:10" ht="15.75">
       <c r="A15" s="5">
         <v>14</v>
       </c>
@@ -5826,7 +8297,7 @@
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
     </row>
-    <row r="16" spans="1:10" ht="15.35">
+    <row r="16" spans="1:10" ht="15.75">
       <c r="A16" s="5">
         <v>15</v>
       </c>
@@ -5848,7 +8319,7 @@
       <c r="I16" s="5"/>
       <c r="J16" s="5"/>
     </row>
-    <row r="17" spans="1:10" ht="15.35">
+    <row r="17" spans="1:10" ht="15.75">
       <c r="A17" s="5">
         <v>16</v>
       </c>
@@ -5870,7 +8341,7 @@
       <c r="I17" s="5"/>
       <c r="J17" s="5"/>
     </row>
-    <row r="18" spans="1:10" ht="15.35">
+    <row r="18" spans="1:10" ht="15.75">
       <c r="A18" s="5">
         <v>17</v>
       </c>
@@ -5892,7 +8363,7 @@
       <c r="I18" s="5"/>
       <c r="J18" s="5"/>
     </row>
-    <row r="19" spans="1:10" ht="15.35">
+    <row r="19" spans="1:10" ht="15.75">
       <c r="A19" s="5">
         <v>18</v>
       </c>
@@ -5914,7 +8385,7 @@
       <c r="I19" s="5"/>
       <c r="J19" s="5"/>
     </row>
-    <row r="20" spans="1:10" ht="15.35">
+    <row r="20" spans="1:10" ht="15.75">
       <c r="A20" s="5">
         <v>19</v>
       </c>
@@ -5936,7 +8407,7 @@
       <c r="I20" s="5"/>
       <c r="J20" s="5"/>
     </row>
-    <row r="21" spans="1:10" ht="15.35">
+    <row r="21" spans="1:10" ht="15.75">
       <c r="A21" s="5">
         <v>20</v>
       </c>
@@ -5958,7 +8429,7 @@
       <c r="I21" s="5"/>
       <c r="J21" s="5"/>
     </row>
-    <row r="22" spans="1:10" ht="15.35">
+    <row r="22" spans="1:10" ht="15.75">
       <c r="A22" s="5"/>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
@@ -5979,24 +8450,24 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M880"/>
   <sheetViews>
     <sheetView topLeftCell="C112" workbookViewId="0">
       <selection activeCell="O42" sqref="O42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.7"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="17.29296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.1171875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.1171875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.41015625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.5859375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.5859375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.41015625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10" bestFit="1" customWidth="1"/>
   </cols>
@@ -6036,7 +8507,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="14.35">
+    <row r="2" spans="1:13" ht="15">
       <c r="A2" s="6">
         <v>4212020070011990</v>
       </c>

</xml_diff>

<commit_message>
Add Exercise 3 Solution
</commit_message>
<xml_diff>
--- a/labs/lab7/Lab7_regression_with_excel.xlsx
+++ b/labs/lab7/Lab7_regression_with_excel.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19995" windowHeight="8880" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19995" windowHeight="8880" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Simple Regression" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1047" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1079" uniqueCount="102">
   <si>
     <t>PRICE</t>
   </si>
@@ -329,6 +329,9 @@
   <si>
     <t>Predicted SALARY (in thousands)</t>
   </si>
+  <si>
+    <t>Predicted Emission</t>
+  </si>
 </sst>
 </file>
 
@@ -967,7 +970,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1307,7 +1309,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -1341,7 +1342,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -2131,7 +2131,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2774,7 +2773,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -2808,7 +2806,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -2822,7 +2819,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -5015,13 +5011,13 @@
       <xdr:rowOff>81915</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>97155</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>428625</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1">
@@ -5036,7 +5032,7 @@
           <xdr:spPr>
             <a:xfrm>
               <a:off x="175260" y="4672965"/>
-              <a:ext cx="3825240" cy="3444240"/>
+              <a:ext cx="3568065" cy="3832860"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -5307,16 +5303,22 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="2" name="TextBox 1"/>
+            <xdr:cNvPr id="2" name="TextBox 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
             <xdr:cNvSpPr txBox="1"/>
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
               <a:off x="175260" y="4672965"/>
-              <a:ext cx="3825240" cy="3444240"/>
+              <a:ext cx="3568065" cy="3832860"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -5420,7 +5422,19 @@
                 <a:rPr lang="en-US" sz="1100" b="0" i="0" baseline="0">
                   <a:latin typeface="Cambria Math"/>
                 </a:rPr>
-                <a:t>𝛽_0   </a:t>
+                <a:t>𝛽</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0" baseline="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>_</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0" baseline="0">
+                  <a:latin typeface="Cambria Math"/>
+                </a:rPr>
+                <a:t>0   </a:t>
               </a:r>
               <a:r>
                 <a:rPr lang="en-US" sz="1100" baseline="0"/>
@@ -5430,7 +5444,19 @@
                 <a:rPr lang="en-US" sz="1100" b="0" i="0" baseline="0">
                   <a:latin typeface="Cambria Math"/>
                 </a:rPr>
-                <a:t>𝛽_1×</a:t>
+                <a:t>𝛽</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0" baseline="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>_</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0" baseline="0">
+                  <a:latin typeface="Cambria Math"/>
+                </a:rPr>
+                <a:t>1×</a:t>
               </a:r>
               <a:r>
                 <a:rPr lang="en-US" sz="1100" baseline="0"/>
@@ -5440,7 +5466,19 @@
                 <a:rPr lang="en-US" sz="1100" b="0" i="0" baseline="0">
                   <a:latin typeface="Cambria Math"/>
                 </a:rPr>
-                <a:t>𝛽_2×</a:t>
+                <a:t>𝛽</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0" baseline="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>_</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0" baseline="0">
+                  <a:latin typeface="Cambria Math"/>
+                </a:rPr>
+                <a:t>2×</a:t>
               </a:r>
               <a:r>
                 <a:rPr lang="en-US" sz="1100"/>
@@ -5450,7 +5488,19 @@
                 <a:rPr lang="en-US" sz="1100" b="0" i="0">
                   <a:latin typeface="Cambria Math"/>
                 </a:rPr>
-                <a:t>𝛽_3×</a:t>
+                <a:t>𝛽</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>_</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math"/>
+                </a:rPr>
+                <a:t>3×</a:t>
               </a:r>
               <a:r>
                 <a:rPr lang="en-US" sz="1100"/>
@@ -5472,7 +5522,7 @@
   </xdr:twoCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>121920</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -5527,16 +5577,16 @@
   </xdr:oneCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>238125</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>104776</xdr:rowOff>
+      <xdr:rowOff>76201</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>323850</xdr:colOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>104776</xdr:rowOff>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -5551,8 +5601,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2943225" y="104776"/>
-          <a:ext cx="5800725" cy="5162550"/>
+          <a:off x="6115050" y="76201"/>
+          <a:ext cx="5915025" cy="5191124"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9545,7 +9595,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q118"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AB50" sqref="AB50"/>
     </sheetView>
   </sheetViews>
@@ -11074,91 +11124,97 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:S75"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L37" sqref="L37"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="U26" sqref="U26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="3.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="9.140625" style="4"/>
-    <col min="9" max="9" width="12.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="4"/>
+    <col min="2" max="2" width="9.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="9.140625" style="4"/>
+    <col min="8" max="8" width="12.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="15" width="9.140625" style="4"/>
+    <col min="16" max="16" width="9.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="6.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75">
+    <row r="1" spans="1:17" ht="15.75">
       <c r="A1" s="10" t="s">
         <v>53</v>
       </c>
       <c r="B1" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="E1" s="10" t="s">
         <v>54</v>
-      </c>
-      <c r="C1" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>57</v>
       </c>
       <c r="F1" s="5"/>
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
       <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-    </row>
-    <row r="2" spans="1:10" ht="15.75">
+      <c r="P1" s="10"/>
+      <c r="Q1" s="10"/>
+    </row>
+    <row r="2" spans="1:17" ht="15.75">
       <c r="A2" s="5">
         <v>1</v>
       </c>
       <c r="B2" s="5">
-        <v>1</v>
+        <v>2.1949999999999998</v>
       </c>
       <c r="C2" s="5">
-        <v>2.1949999999999998</v>
+        <v>14.2683</v>
       </c>
       <c r="D2" s="5">
-        <v>14.2683</v>
+        <v>18.2927</v>
       </c>
       <c r="E2" s="5">
-        <v>18.2927</v>
+        <v>1</v>
       </c>
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-    </row>
-    <row r="3" spans="1:10" ht="15.75">
+      <c r="P2" s="5"/>
+      <c r="Q2" s="5"/>
+    </row>
+    <row r="3" spans="1:17" ht="15.75">
       <c r="A3" s="5">
         <v>2</v>
       </c>
       <c r="B3" s="5">
-        <v>1</v>
+        <v>1.756</v>
       </c>
       <c r="C3" s="5">
-        <v>1.756</v>
+        <v>14.333299999999999</v>
       </c>
       <c r="D3" s="5">
-        <v>14.333299999999999</v>
+        <v>18.488900000000001</v>
       </c>
       <c r="E3" s="5">
-        <v>18.488900000000001</v>
+        <v>1</v>
       </c>
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-    </row>
-    <row r="4" spans="1:10" ht="15.75">
+      <c r="P3" s="5"/>
+      <c r="Q3" s="5"/>
+    </row>
+    <row r="4" spans="1:17" ht="15.75">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -11166,197 +11222,206 @@
         <v>1</v>
       </c>
       <c r="C4" s="5">
-        <v>1</v>
+        <v>13.875</v>
       </c>
       <c r="D4" s="5">
-        <v>13.875</v>
+        <v>18.125</v>
       </c>
       <c r="E4" s="5">
-        <v>18.125</v>
+        <v>1</v>
       </c>
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-    </row>
-    <row r="5" spans="1:10" ht="15.75">
+      <c r="P4" s="5"/>
+      <c r="Q4" s="5"/>
+    </row>
+    <row r="5" spans="1:17" ht="15.75">
       <c r="A5" s="5">
         <v>4</v>
       </c>
       <c r="B5" s="5">
+        <v>7</v>
+      </c>
+      <c r="C5" s="5">
+        <v>21.5</v>
+      </c>
+      <c r="D5" s="5">
+        <v>30.25</v>
+      </c>
+      <c r="E5" s="5">
         <v>5</v>
-      </c>
-      <c r="C5" s="5">
-        <v>7</v>
-      </c>
-      <c r="D5" s="5">
-        <v>21.5</v>
-      </c>
-      <c r="E5" s="5">
-        <v>30.25</v>
       </c>
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-    </row>
-    <row r="6" spans="1:10" ht="15.75">
+      <c r="P5" s="5"/>
+      <c r="Q5" s="5"/>
+    </row>
+    <row r="6" spans="1:17" ht="15.75">
       <c r="A6" s="5">
         <v>5</v>
       </c>
       <c r="B6" s="5">
+        <v>8.3079999999999998</v>
+      </c>
+      <c r="C6" s="5">
+        <v>22.384599999999999</v>
+      </c>
+      <c r="D6" s="5">
+        <v>31.538499999999999</v>
+      </c>
+      <c r="E6" s="5">
         <v>5</v>
-      </c>
-      <c r="C6" s="5">
-        <v>8.3079999999999998</v>
-      </c>
-      <c r="D6" s="5">
-        <v>22.384599999999999</v>
-      </c>
-      <c r="E6" s="5">
-        <v>31.538499999999999</v>
       </c>
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
-    </row>
-    <row r="7" spans="1:10" ht="15.75">
+      <c r="P6" s="5"/>
+      <c r="Q6" s="5"/>
+    </row>
+    <row r="7" spans="1:17" ht="15.75">
       <c r="A7" s="5">
         <v>6</v>
       </c>
       <c r="B7" s="5">
+        <v>4</v>
+      </c>
+      <c r="C7" s="5">
+        <v>15.416700000000001</v>
+      </c>
+      <c r="D7" s="5">
+        <v>19.916699999999999</v>
+      </c>
+      <c r="E7" s="5">
         <v>3</v>
-      </c>
-      <c r="C7" s="5">
-        <v>4</v>
-      </c>
-      <c r="D7" s="5">
-        <v>15.416700000000001</v>
-      </c>
-      <c r="E7" s="5">
-        <v>19.916699999999999</v>
       </c>
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
       <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
-    </row>
-    <row r="8" spans="1:10" ht="15.75">
+      <c r="P7" s="5"/>
+      <c r="Q7" s="5"/>
+    </row>
+    <row r="8" spans="1:17" ht="15.75">
       <c r="A8" s="5">
         <v>7</v>
       </c>
       <c r="B8" s="5">
+        <v>5.6</v>
+      </c>
+      <c r="C8" s="5">
+        <v>26.8</v>
+      </c>
+      <c r="D8" s="5">
+        <v>32</v>
+      </c>
+      <c r="E8" s="5">
         <v>6</v>
-      </c>
-      <c r="C8" s="5">
-        <v>5.6</v>
-      </c>
-      <c r="D8" s="5">
-        <v>26.8</v>
-      </c>
-      <c r="E8" s="5">
-        <v>32</v>
       </c>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
       <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
-    </row>
-    <row r="9" spans="1:10" ht="15.75">
+      <c r="P8" s="5"/>
+      <c r="Q8" s="5"/>
+    </row>
+    <row r="9" spans="1:17" ht="15.75">
       <c r="A9" s="5">
         <v>8</v>
       </c>
       <c r="B9" s="5">
+        <v>6.5</v>
+      </c>
+      <c r="C9" s="5">
+        <v>19.5</v>
+      </c>
+      <c r="D9" s="5">
+        <v>26.75</v>
+      </c>
+      <c r="E9" s="5">
         <v>4</v>
-      </c>
-      <c r="C9" s="5">
-        <v>6.5</v>
-      </c>
-      <c r="D9" s="5">
-        <v>19.5</v>
-      </c>
-      <c r="E9" s="5">
-        <v>26.75</v>
       </c>
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
       <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
-    </row>
-    <row r="10" spans="1:10" ht="15.75">
+      <c r="P9" s="5"/>
+      <c r="Q9" s="5"/>
+    </row>
+    <row r="10" spans="1:17" ht="15.75">
       <c r="A10" s="5">
         <v>9</v>
       </c>
       <c r="B10" s="5">
+        <v>7.8</v>
+      </c>
+      <c r="C10" s="5">
+        <v>30.6</v>
+      </c>
+      <c r="D10" s="5">
+        <v>36.4</v>
+      </c>
+      <c r="E10" s="5">
         <v>6</v>
-      </c>
-      <c r="C10" s="5">
-        <v>7.8</v>
-      </c>
-      <c r="D10" s="5">
-        <v>30.6</v>
-      </c>
-      <c r="E10" s="5">
-        <v>36.4</v>
       </c>
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
       <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
-    </row>
-    <row r="11" spans="1:10" ht="15.75">
+      <c r="P10" s="5"/>
+      <c r="Q10" s="5"/>
+    </row>
+    <row r="11" spans="1:17" ht="15.75">
       <c r="A11" s="5">
         <v>10</v>
       </c>
       <c r="B11" s="5">
+        <v>6.6</v>
+      </c>
+      <c r="C11" s="5">
+        <v>19.600000000000001</v>
+      </c>
+      <c r="D11" s="5">
+        <v>30</v>
+      </c>
+      <c r="E11" s="5">
         <v>4</v>
-      </c>
-      <c r="C11" s="5">
-        <v>6.6</v>
-      </c>
-      <c r="D11" s="5">
-        <v>19.600000000000001</v>
-      </c>
-      <c r="E11" s="5">
-        <v>30</v>
       </c>
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
-      <c r="J11" s="5"/>
-    </row>
-    <row r="12" spans="1:10" ht="15.75">
+      <c r="P11" s="5"/>
+      <c r="Q11" s="5"/>
+    </row>
+    <row r="12" spans="1:17" ht="15.75">
       <c r="A12" s="5">
         <v>11</v>
       </c>
       <c r="B12" s="5">
+        <v>2.3330000000000002</v>
+      </c>
+      <c r="C12" s="5">
+        <v>14.833299999999999</v>
+      </c>
+      <c r="D12" s="5">
+        <v>19.5</v>
+      </c>
+      <c r="E12" s="5">
         <v>3</v>
-      </c>
-      <c r="C12" s="5">
-        <v>2.3330000000000002</v>
-      </c>
-      <c r="D12" s="5">
-        <v>14.833299999999999</v>
-      </c>
-      <c r="E12" s="5">
-        <v>19.5</v>
       </c>
       <c r="F12" s="5"/>
       <c r="G12" s="5"/>
       <c r="H12" s="5"/>
       <c r="I12" s="5"/>
-      <c r="J12" s="5"/>
-    </row>
-    <row r="13" spans="1:10" ht="15.75">
+      <c r="P12" s="5"/>
+      <c r="Q12" s="5"/>
+    </row>
+    <row r="13" spans="1:17" ht="15.75">
       <c r="A13" s="5">
         <v>12</v>
       </c>
@@ -11364,175 +11429,183 @@
         <v>6</v>
       </c>
       <c r="C13" s="5">
+        <v>25</v>
+      </c>
+      <c r="D13" s="5">
+        <v>33</v>
+      </c>
+      <c r="E13" s="5">
         <v>6</v>
-      </c>
-      <c r="D13" s="5">
-        <v>25</v>
-      </c>
-      <c r="E13" s="5">
-        <v>33</v>
       </c>
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
       <c r="I13" s="5"/>
-      <c r="J13" s="5"/>
-    </row>
-    <row r="14" spans="1:10" ht="15.75">
+      <c r="P13" s="5"/>
+      <c r="Q13" s="5"/>
+    </row>
+    <row r="14" spans="1:17" ht="15.75">
       <c r="A14" s="5">
         <v>13</v>
       </c>
       <c r="B14" s="5">
+        <v>4</v>
+      </c>
+      <c r="C14" s="5">
+        <v>18.666699999999999</v>
+      </c>
+      <c r="D14" s="5">
+        <v>25</v>
+      </c>
+      <c r="E14" s="5">
         <v>2</v>
-      </c>
-      <c r="C14" s="5">
-        <v>4</v>
-      </c>
-      <c r="D14" s="5">
-        <v>18.666699999999999</v>
-      </c>
-      <c r="E14" s="5">
-        <v>25</v>
       </c>
       <c r="F14" s="5"/>
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
-      <c r="J14" s="5"/>
-    </row>
-    <row r="15" spans="1:10" ht="15.75">
+      <c r="P14" s="5"/>
+      <c r="Q14" s="5"/>
+    </row>
+    <row r="15" spans="1:17" ht="15.75">
       <c r="A15" s="5">
         <v>14</v>
       </c>
       <c r="B15" s="5">
+        <v>7.8460000000000001</v>
+      </c>
+      <c r="C15" s="5">
+        <v>25.1538</v>
+      </c>
+      <c r="D15" s="5">
+        <v>31.769200000000001</v>
+      </c>
+      <c r="E15" s="5">
         <v>6</v>
-      </c>
-      <c r="C15" s="5">
-        <v>7.8460000000000001</v>
-      </c>
-      <c r="D15" s="5">
-        <v>25.1538</v>
-      </c>
-      <c r="E15" s="5">
-        <v>31.769200000000001</v>
       </c>
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
-      <c r="J15" s="5"/>
-    </row>
-    <row r="16" spans="1:10" ht="15.75">
+      <c r="P15" s="5"/>
+      <c r="Q15" s="5"/>
+    </row>
+    <row r="16" spans="1:17" ht="15.75">
       <c r="A16" s="5">
         <v>15</v>
       </c>
       <c r="B16" s="5">
-        <v>1</v>
+        <v>4.8330000000000002</v>
       </c>
       <c r="C16" s="5">
-        <v>4.8330000000000002</v>
+        <v>17.916699999999999</v>
       </c>
       <c r="D16" s="5">
-        <v>17.916699999999999</v>
+        <v>22.166699999999999</v>
       </c>
       <c r="E16" s="5">
-        <v>22.166699999999999</v>
+        <v>1</v>
       </c>
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
       <c r="I16" s="5"/>
-      <c r="J16" s="5"/>
-    </row>
-    <row r="17" spans="1:10" ht="15.75">
+      <c r="P16" s="5"/>
+      <c r="Q16" s="5"/>
+    </row>
+    <row r="17" spans="1:19" ht="15.75">
       <c r="A17" s="5">
         <v>16</v>
       </c>
       <c r="B17" s="5">
+        <v>6.5</v>
+      </c>
+      <c r="C17" s="5">
+        <v>21.5</v>
+      </c>
+      <c r="D17" s="5">
+        <v>27.5</v>
+      </c>
+      <c r="E17" s="5">
         <v>5</v>
-      </c>
-      <c r="C17" s="5">
-        <v>6.5</v>
-      </c>
-      <c r="D17" s="5">
-        <v>21.5</v>
-      </c>
-      <c r="E17" s="5">
-        <v>27.5</v>
       </c>
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
       <c r="I17" s="5"/>
-      <c r="J17" s="5"/>
-    </row>
-    <row r="18" spans="1:10" ht="15.75">
+      <c r="P17" s="5"/>
+      <c r="Q17" s="5"/>
+    </row>
+    <row r="18" spans="1:19" ht="15.75">
       <c r="A18" s="5">
         <v>17</v>
       </c>
       <c r="B18" s="5">
+        <v>1.4</v>
+      </c>
+      <c r="C18" s="5">
+        <v>13.8</v>
+      </c>
+      <c r="D18" s="5">
+        <v>17.8</v>
+      </c>
+      <c r="E18" s="5">
         <v>3</v>
-      </c>
-      <c r="C18" s="5">
-        <v>1.4</v>
-      </c>
-      <c r="D18" s="5">
-        <v>13.8</v>
-      </c>
-      <c r="E18" s="5">
-        <v>17.8</v>
       </c>
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
       <c r="H18" s="5"/>
       <c r="I18" s="5"/>
-      <c r="J18" s="5"/>
-    </row>
-    <row r="19" spans="1:10" ht="15.75">
+      <c r="P18" s="5"/>
+      <c r="Q18" s="5"/>
+    </row>
+    <row r="19" spans="1:19" ht="15.75">
       <c r="A19" s="5">
         <v>18</v>
       </c>
       <c r="B19" s="5">
-        <v>1</v>
+        <v>1.7729999999999999</v>
       </c>
       <c r="C19" s="5">
-        <v>1.7729999999999999</v>
+        <v>14.5227</v>
       </c>
       <c r="D19" s="5">
-        <v>14.5227</v>
+        <v>18.590900000000001</v>
       </c>
       <c r="E19" s="5">
-        <v>18.590900000000001</v>
+        <v>1</v>
       </c>
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
       <c r="H19" s="5"/>
       <c r="I19" s="5"/>
-      <c r="J19" s="5"/>
-    </row>
-    <row r="20" spans="1:10" ht="15.75">
+      <c r="P19" s="5"/>
+      <c r="Q19" s="5"/>
+    </row>
+    <row r="20" spans="1:19" ht="15.75">
       <c r="A20" s="5">
         <v>19</v>
       </c>
       <c r="B20" s="5">
+        <v>5</v>
+      </c>
+      <c r="C20" s="5">
+        <v>15.5</v>
+      </c>
+      <c r="D20" s="5">
+        <v>20.5</v>
+      </c>
+      <c r="E20" s="5">
         <v>3</v>
-      </c>
-      <c r="C20" s="5">
-        <v>5</v>
-      </c>
-      <c r="D20" s="5">
-        <v>15.5</v>
-      </c>
-      <c r="E20" s="5">
-        <v>20.5</v>
       </c>
       <c r="F20" s="5"/>
       <c r="G20" s="5"/>
       <c r="H20" s="5"/>
       <c r="I20" s="5"/>
-      <c r="J20" s="5"/>
-    </row>
-    <row r="21" spans="1:10" ht="15.75">
+      <c r="P20" s="5"/>
+      <c r="Q20" s="5"/>
+    </row>
+    <row r="21" spans="1:19" ht="15.75">
       <c r="A21" s="5">
         <v>20</v>
       </c>
@@ -11540,21 +11613,22 @@
         <v>3</v>
       </c>
       <c r="C21" s="5">
+        <v>13.5</v>
+      </c>
+      <c r="D21" s="5">
+        <v>18</v>
+      </c>
+      <c r="E21" s="5">
         <v>3</v>
-      </c>
-      <c r="D21" s="5">
-        <v>13.5</v>
-      </c>
-      <c r="E21" s="5">
-        <v>18</v>
       </c>
       <c r="F21" s="5"/>
       <c r="G21" s="5"/>
       <c r="H21" s="5"/>
       <c r="I21" s="5"/>
-      <c r="J21" s="5"/>
-    </row>
-    <row r="22" spans="1:10" ht="15.75">
+      <c r="P21" s="5"/>
+      <c r="Q21" s="5"/>
+    </row>
+    <row r="22" spans="1:19" ht="15.75">
       <c r="A22" s="5"/>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
@@ -11564,13 +11638,799 @@
       <c r="G22" s="5"/>
       <c r="H22" s="5"/>
       <c r="I22" s="5"/>
-      <c r="J22" s="5"/>
+      <c r="P22" s="5"/>
+      <c r="Q22" s="5"/>
+    </row>
+    <row r="30" spans="1:19">
+      <c r="K30" t="s">
+        <v>72</v>
+      </c>
+      <c r="L30"/>
+      <c r="M30"/>
+      <c r="N30"/>
+      <c r="O30"/>
+      <c r="P30"/>
+      <c r="Q30"/>
+      <c r="R30"/>
+      <c r="S30"/>
+    </row>
+    <row r="31" spans="1:19" ht="15.75" thickBot="1">
+      <c r="K31"/>
+      <c r="L31"/>
+      <c r="M31"/>
+      <c r="N31"/>
+      <c r="O31"/>
+      <c r="P31"/>
+      <c r="Q31"/>
+      <c r="R31"/>
+      <c r="S31"/>
+    </row>
+    <row r="32" spans="1:19">
+      <c r="K32" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="L32" s="16"/>
+      <c r="M32"/>
+      <c r="N32"/>
+      <c r="O32"/>
+      <c r="P32"/>
+      <c r="Q32"/>
+      <c r="R32"/>
+      <c r="S32"/>
+    </row>
+    <row r="33" spans="11:19">
+      <c r="K33" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="L33" s="13">
+        <v>0.91453436292771384</v>
+      </c>
+      <c r="M33"/>
+      <c r="N33"/>
+      <c r="O33"/>
+      <c r="P33"/>
+      <c r="Q33"/>
+      <c r="R33"/>
+      <c r="S33"/>
+    </row>
+    <row r="34" spans="11:19">
+      <c r="K34" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="L34" s="13">
+        <v>0.83637310097559936</v>
+      </c>
+      <c r="M34"/>
+      <c r="N34"/>
+      <c r="O34"/>
+      <c r="P34"/>
+      <c r="Q34"/>
+      <c r="R34"/>
+      <c r="S34"/>
+    </row>
+    <row r="35" spans="11:19">
+      <c r="K35" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="L35" s="13">
+        <v>0.80569305740852426</v>
+      </c>
+      <c r="M35"/>
+      <c r="N35"/>
+      <c r="O35"/>
+      <c r="P35"/>
+      <c r="Q35"/>
+      <c r="R35"/>
+      <c r="S35"/>
+    </row>
+    <row r="36" spans="11:19">
+      <c r="K36" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="L36" s="13">
+        <v>1.0512321072353801</v>
+      </c>
+      <c r="M36"/>
+      <c r="N36"/>
+      <c r="O36"/>
+      <c r="P36"/>
+      <c r="Q36"/>
+      <c r="R36"/>
+      <c r="S36"/>
+    </row>
+    <row r="37" spans="11:19" ht="15.75" thickBot="1">
+      <c r="K37" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="L37" s="14">
+        <v>20</v>
+      </c>
+      <c r="M37"/>
+      <c r="N37"/>
+      <c r="O37"/>
+      <c r="P37"/>
+      <c r="Q37"/>
+      <c r="R37"/>
+      <c r="S37"/>
+    </row>
+    <row r="38" spans="11:19">
+      <c r="K38"/>
+      <c r="L38"/>
+      <c r="M38"/>
+      <c r="N38"/>
+      <c r="O38"/>
+      <c r="P38"/>
+      <c r="Q38"/>
+      <c r="R38"/>
+      <c r="S38"/>
+    </row>
+    <row r="39" spans="11:19" ht="15.75" thickBot="1">
+      <c r="K39" t="s">
+        <v>79</v>
+      </c>
+      <c r="L39"/>
+      <c r="M39"/>
+      <c r="N39"/>
+      <c r="O39"/>
+      <c r="P39"/>
+      <c r="Q39"/>
+      <c r="R39"/>
+      <c r="S39"/>
+    </row>
+    <row r="40" spans="11:19">
+      <c r="K40" s="15"/>
+      <c r="L40" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="M40" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="N40" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="O40" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="P40" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q40"/>
+      <c r="R40"/>
+      <c r="S40"/>
+    </row>
+    <row r="41" spans="11:19">
+      <c r="K41" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="L41" s="13">
+        <v>3</v>
+      </c>
+      <c r="M41" s="13">
+        <v>90.377968107479376</v>
+      </c>
+      <c r="N41" s="13">
+        <v>30.125989369159793</v>
+      </c>
+      <c r="O41" s="13">
+        <v>27.261144500888822</v>
+      </c>
+      <c r="P41" s="13">
+        <v>1.5857526871156119E-6</v>
+      </c>
+      <c r="Q41"/>
+      <c r="R41"/>
+      <c r="S41"/>
+    </row>
+    <row r="42" spans="11:19">
+      <c r="K42" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="L42" s="13">
+        <v>16</v>
+      </c>
+      <c r="M42" s="13">
+        <v>17.681423092520603</v>
+      </c>
+      <c r="N42" s="13">
+        <v>1.1050889432825377</v>
+      </c>
+      <c r="O42" s="13"/>
+      <c r="P42" s="13"/>
+      <c r="Q42"/>
+      <c r="R42"/>
+      <c r="S42"/>
+    </row>
+    <row r="43" spans="11:19" ht="15.75" thickBot="1">
+      <c r="K43" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="L43" s="14">
+        <v>19</v>
+      </c>
+      <c r="M43" s="14">
+        <v>108.05939119999998</v>
+      </c>
+      <c r="N43" s="14"/>
+      <c r="O43" s="14"/>
+      <c r="P43" s="14"/>
+      <c r="Q43"/>
+      <c r="R43"/>
+      <c r="S43"/>
+    </row>
+    <row r="44" spans="11:19" ht="15.75" thickBot="1">
+      <c r="K44"/>
+      <c r="L44"/>
+      <c r="M44"/>
+      <c r="N44"/>
+      <c r="O44"/>
+      <c r="P44"/>
+      <c r="Q44"/>
+      <c r="R44"/>
+      <c r="S44"/>
+    </row>
+    <row r="45" spans="11:19">
+      <c r="K45" s="15"/>
+      <c r="L45" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="M45" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="N45" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="O45" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="P45" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q45" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="R45" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="S45" s="15" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="46" spans="11:19">
+      <c r="K46" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="L46" s="13">
+        <v>-3.2393462446325825</v>
+      </c>
+      <c r="M46" s="13">
+        <v>1.2496484614647325</v>
+      </c>
+      <c r="N46" s="13">
+        <v>-2.5922060039474575</v>
+      </c>
+      <c r="O46" s="13">
+        <v>1.964931507749797E-2</v>
+      </c>
+      <c r="P46" s="13">
+        <v>-5.8884826402553578</v>
+      </c>
+      <c r="Q46" s="13">
+        <v>-0.59020984900980755</v>
+      </c>
+      <c r="R46" s="13">
+        <v>-5.8884826402553578</v>
+      </c>
+      <c r="S46" s="13">
+        <v>-0.59020984900980755</v>
+      </c>
+    </row>
+    <row r="47" spans="11:19">
+      <c r="K47" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="L47" s="13">
+        <v>-0.27338273679575442</v>
+      </c>
+      <c r="M47" s="13">
+        <v>0.18306433644808906</v>
+      </c>
+      <c r="N47" s="13">
+        <v>-1.4933697196301075</v>
+      </c>
+      <c r="O47" s="13">
+        <v>0.15479761584706503</v>
+      </c>
+      <c r="P47" s="13">
+        <v>-0.6614617937304812</v>
+      </c>
+      <c r="Q47" s="13">
+        <v>0.1146963201389723</v>
+      </c>
+      <c r="R47" s="13">
+        <v>-0.6614617937304812</v>
+      </c>
+      <c r="S47" s="13">
+        <v>0.1146963201389723</v>
+      </c>
+    </row>
+    <row r="48" spans="11:19">
+      <c r="K48" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="L48" s="13">
+        <v>0.49999912639378968</v>
+      </c>
+      <c r="M48" s="13">
+        <v>0.15609444237458922</v>
+      </c>
+      <c r="N48" s="13">
+        <v>3.2031833983807809</v>
+      </c>
+      <c r="O48" s="13">
+        <v>5.5405147390915873E-3</v>
+      </c>
+      <c r="P48" s="13">
+        <v>0.16909369082491116</v>
+      </c>
+      <c r="Q48" s="13">
+        <v>0.83090456196266826</v>
+      </c>
+      <c r="R48" s="13">
+        <v>0.16909369082491116</v>
+      </c>
+      <c r="S48" s="13">
+        <v>0.83090456196266826</v>
+      </c>
+    </row>
+    <row r="49" spans="11:19" ht="15.75" thickBot="1">
+      <c r="K49" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="L49" s="14">
+        <v>0.20230723920853944</v>
+      </c>
+      <c r="M49" s="14">
+        <v>0.26219317727706837</v>
+      </c>
+      <c r="N49" s="14">
+        <v>0.77159612355112717</v>
+      </c>
+      <c r="O49" s="14">
+        <v>0.4515998062704939</v>
+      </c>
+      <c r="P49" s="14">
+        <v>-0.35351746672077577</v>
+      </c>
+      <c r="Q49" s="14">
+        <v>0.75813194513785465</v>
+      </c>
+      <c r="R49" s="14">
+        <v>-0.35351746672077577</v>
+      </c>
+      <c r="S49" s="14">
+        <v>0.75813194513785465</v>
+      </c>
+    </row>
+    <row r="50" spans="11:19">
+      <c r="K50"/>
+      <c r="L50"/>
+      <c r="M50"/>
+      <c r="N50"/>
+      <c r="O50"/>
+      <c r="P50"/>
+      <c r="Q50"/>
+      <c r="R50"/>
+      <c r="S50"/>
+    </row>
+    <row r="51" spans="11:19">
+      <c r="K51"/>
+      <c r="L51"/>
+      <c r="M51"/>
+      <c r="N51"/>
+      <c r="O51"/>
+      <c r="P51"/>
+      <c r="Q51"/>
+      <c r="R51"/>
+      <c r="S51"/>
+    </row>
+    <row r="52" spans="11:19">
+      <c r="K52"/>
+      <c r="L52"/>
+      <c r="M52"/>
+      <c r="N52"/>
+      <c r="O52"/>
+      <c r="P52"/>
+      <c r="Q52"/>
+      <c r="R52"/>
+      <c r="S52"/>
+    </row>
+    <row r="53" spans="11:19">
+      <c r="K53" t="s">
+        <v>96</v>
+      </c>
+      <c r="L53"/>
+      <c r="M53"/>
+      <c r="N53"/>
+      <c r="O53"/>
+      <c r="P53"/>
+      <c r="Q53"/>
+      <c r="R53"/>
+      <c r="S53"/>
+    </row>
+    <row r="54" spans="11:19" ht="15.75" thickBot="1">
+      <c r="K54"/>
+      <c r="L54"/>
+      <c r="M54"/>
+      <c r="N54"/>
+      <c r="O54"/>
+      <c r="P54"/>
+      <c r="Q54"/>
+      <c r="R54"/>
+      <c r="S54"/>
+    </row>
+    <row r="55" spans="11:19">
+      <c r="K55" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="L55" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="M55" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="N55"/>
+      <c r="O55"/>
+      <c r="P55"/>
+      <c r="Q55"/>
+      <c r="R55"/>
+      <c r="S55"/>
+    </row>
+    <row r="56" spans="11:19">
+      <c r="K56" s="13">
+        <v>1</v>
+      </c>
+      <c r="L56" s="13">
+        <v>2.2085881105367706</v>
+      </c>
+      <c r="M56" s="13">
+        <v>-1.3588110536770781E-2</v>
+      </c>
+      <c r="N56"/>
+      <c r="O56"/>
+      <c r="P56"/>
+      <c r="Q56"/>
+      <c r="R56"/>
+      <c r="S56"/>
+    </row>
+    <row r="57" spans="11:19">
+      <c r="K57" s="13">
+        <v>2</v>
+      </c>
+      <c r="L57" s="13">
+        <v>2.2889180612435087</v>
+      </c>
+      <c r="M57" s="13">
+        <v>-0.53291806124350871</v>
+      </c>
+      <c r="N57"/>
+      <c r="O57"/>
+      <c r="P57"/>
+      <c r="Q57"/>
+      <c r="R57"/>
+      <c r="S57"/>
+    </row>
+    <row r="58" spans="11:19">
+      <c r="K58" s="13">
+        <v>3</v>
+      </c>
+      <c r="L58" s="13">
+        <v>2.2322596874223022</v>
+      </c>
+      <c r="M58" s="13">
+        <v>-1.2322596874223022</v>
+      </c>
+      <c r="N58"/>
+      <c r="O58"/>
+      <c r="P58"/>
+      <c r="Q58"/>
+      <c r="R58"/>
+      <c r="S58"/>
+    </row>
+    <row r="59" spans="11:19">
+      <c r="K59" s="13">
+        <v>4</v>
+      </c>
+      <c r="L59" s="13">
+        <v>7.0194346837135333</v>
+      </c>
+      <c r="M59" s="13">
+        <v>-1.9434683713533296E-2</v>
+      </c>
+      <c r="N59"/>
+      <c r="O59"/>
+      <c r="P59"/>
+      <c r="Q59"/>
+      <c r="R59"/>
+      <c r="S59"/>
+    </row>
+    <row r="60" spans="11:19">
+      <c r="K60" s="13">
+        <v>5</v>
+      </c>
+      <c r="L60" s="13">
+        <v>7.4218491891024074</v>
+      </c>
+      <c r="M60" s="13">
+        <v>0.8861508108975924</v>
+      </c>
+      <c r="N60"/>
+      <c r="O60"/>
+      <c r="P60"/>
+      <c r="Q60"/>
+      <c r="R60"/>
+      <c r="S60"/>
+    </row>
+    <row r="61" spans="11:19">
+      <c r="K61" s="13">
+        <v>6</v>
+      </c>
+      <c r="L61" s="13">
+        <v>3.1112484352811203</v>
+      </c>
+      <c r="M61" s="13">
+        <v>0.88875156471887973</v>
+      </c>
+      <c r="N61"/>
+      <c r="O61"/>
+      <c r="P61"/>
+      <c r="Q61"/>
+      <c r="R61"/>
+      <c r="S61"/>
+    </row>
+    <row r="62" spans="11:19">
+      <c r="K62" s="13">
+        <v>7</v>
+      </c>
+      <c r="L62" s="13">
+        <v>6.6478118890937061</v>
+      </c>
+      <c r="M62" s="13">
+        <v>-1.0478118890937065</v>
+      </c>
+      <c r="N62"/>
+      <c r="O62"/>
+      <c r="P62"/>
+      <c r="Q62"/>
+      <c r="R62"/>
+      <c r="S62"/>
+    </row>
+    <row r="63" spans="11:19">
+      <c r="K63" s="13">
+        <v>8</v>
+      </c>
+      <c r="L63" s="13">
+        <v>5.6138959757182381</v>
+      </c>
+      <c r="M63" s="13">
+        <v>0.88610402428176194</v>
+      </c>
+      <c r="N63"/>
+      <c r="O63"/>
+      <c r="P63"/>
+      <c r="Q63"/>
+      <c r="R63"/>
+      <c r="S63"/>
+    </row>
+    <row r="64" spans="11:19">
+      <c r="K64" s="13">
+        <v>9</v>
+      </c>
+      <c r="L64" s="13">
+        <v>7.8089536454025144</v>
+      </c>
+      <c r="M64" s="13">
+        <v>-8.9536454025145318E-3</v>
+      </c>
+      <c r="N64"/>
+      <c r="O64"/>
+      <c r="P64"/>
+      <c r="Q64"/>
+      <c r="R64"/>
+      <c r="S64"/>
+    </row>
+    <row r="65" spans="11:19">
+      <c r="K65" s="13">
+        <v>10</v>
+      </c>
+      <c r="L65" s="13">
+        <v>7.2115548628184794</v>
+      </c>
+      <c r="M65" s="13">
+        <v>-0.61155486281847971</v>
+      </c>
+      <c r="N65"/>
+      <c r="O65"/>
+      <c r="P65"/>
+      <c r="Q65"/>
+      <c r="R65"/>
+      <c r="S65"/>
+    </row>
+    <row r="66" spans="11:19">
+      <c r="K66" s="13">
+        <v>11</v>
+      </c>
+      <c r="L66" s="13">
+        <v>3.0623902879594711</v>
+      </c>
+      <c r="M66" s="13">
+        <v>-0.72939028795947092</v>
+      </c>
+      <c r="N66"/>
+      <c r="O66"/>
+      <c r="P66"/>
+      <c r="Q66"/>
+      <c r="R66"/>
+      <c r="S66"/>
+    </row>
+    <row r="67" spans="11:19">
+      <c r="K67" s="13">
+        <v>12</v>
+      </c>
+      <c r="L67" s="13">
+        <v>7.6398999417198539</v>
+      </c>
+      <c r="M67" s="13">
+        <v>-1.6398999417198539</v>
+      </c>
+      <c r="N67"/>
+      <c r="O67"/>
+      <c r="P67"/>
+      <c r="Q67"/>
+      <c r="R67"/>
+      <c r="S67"/>
+    </row>
+    <row r="68" spans="11:19">
+      <c r="K68" s="13">
+        <v>13</v>
+      </c>
+      <c r="L68" s="13">
+        <v>4.5620928606839293</v>
+      </c>
+      <c r="M68" s="13">
+        <v>-0.56209286068392927</v>
+      </c>
+      <c r="N68"/>
+      <c r="O68"/>
+      <c r="P68"/>
+      <c r="Q68"/>
+      <c r="R68"/>
+      <c r="S68"/>
+    </row>
+    <row r="69" spans="11:19">
+      <c r="K69" s="13">
+        <v>14</v>
+      </c>
+      <c r="L69" s="13">
+        <v>6.9824547520351903</v>
+      </c>
+      <c r="M69" s="13">
+        <v>0.8635452479648098</v>
+      </c>
+      <c r="N69"/>
+      <c r="O69"/>
+      <c r="P69"/>
+      <c r="Q69"/>
+      <c r="R69"/>
+      <c r="S69"/>
+    </row>
+    <row r="70" spans="11:19">
+      <c r="K70" s="13">
+        <v>15</v>
+      </c>
+      <c r="L70" s="13">
+        <v>3.1481751492606813</v>
+      </c>
+      <c r="M70" s="13">
+        <v>1.6848248507393189</v>
+      </c>
+      <c r="N70"/>
+      <c r="O70"/>
+      <c r="P70"/>
+      <c r="Q70"/>
+      <c r="R70"/>
+      <c r="S70"/>
+    </row>
+    <row r="71" spans="11:19">
+      <c r="K71" s="13">
+        <v>16</v>
+      </c>
+      <c r="L71" s="13">
+        <v>5.644437086130611</v>
+      </c>
+      <c r="M71" s="13">
+        <v>0.85556291386938899</v>
+      </c>
+      <c r="N71"/>
+      <c r="O71"/>
+      <c r="P71"/>
+      <c r="Q71"/>
+      <c r="R71"/>
+      <c r="S71"/>
+    </row>
+    <row r="72" spans="11:19">
+      <c r="K72" s="13">
+        <v>17</v>
+      </c>
+      <c r="L72" s="13">
+        <v>2.4948781550210812</v>
+      </c>
+      <c r="M72" s="13">
+        <v>-1.0948781550210813</v>
+      </c>
+      <c r="N72"/>
+      <c r="O72"/>
+      <c r="P72"/>
+      <c r="Q72"/>
+      <c r="R72"/>
+      <c r="S72"/>
+    </row>
+    <row r="73" spans="11:19">
+      <c r="K73" s="13">
+        <v>18</v>
+      </c>
+      <c r="L73" s="13">
+        <v>2.2881392817865587</v>
+      </c>
+      <c r="M73" s="13">
+        <v>-0.51513928178655877</v>
+      </c>
+      <c r="N73"/>
+      <c r="O73"/>
+      <c r="P73"/>
+      <c r="Q73"/>
+      <c r="R73"/>
+      <c r="S73"/>
+    </row>
+    <row r="74" spans="11:19">
+      <c r="K74" s="13">
+        <v>19</v>
+      </c>
+      <c r="L74" s="13">
+        <v>3.3801251437315303</v>
+      </c>
+      <c r="M74" s="13">
+        <v>1.6198748562684697</v>
+      </c>
+      <c r="N74"/>
+      <c r="O74"/>
+      <c r="P74"/>
+      <c r="Q74"/>
+      <c r="R74"/>
+      <c r="S74"/>
+    </row>
+    <row r="75" spans="11:19" ht="15.75" thickBot="1">
+      <c r="K75" s="14">
+        <v>20</v>
+      </c>
+      <c r="L75" s="14">
+        <v>2.6768928013385667</v>
+      </c>
+      <c r="M75" s="14">
+        <v>0.32310719866143334</v>
+      </c>
+      <c r="N75"/>
+      <c r="O75"/>
+      <c r="P75"/>
+      <c r="Q75"/>
+      <c r="R75"/>
+      <c r="S75"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>